<commit_message>
modify 0328 add the function of B Field View
</commit_message>
<xml_diff>
--- a/diagnostics/emd/data/EXL50U coefficient.xlsx
+++ b/diagnostics/emd/data/EXL50U coefficient.xlsx
@@ -446,10 +446,10 @@
     <t>Flux032</t>
   </si>
   <si>
+    <t>Flux033</t>
+  </si>
+  <si>
     <t>环电压</t>
-  </si>
-  <si>
-    <t>Flux033</t>
   </si>
   <si>
     <t>Flux034</t>
@@ -783,7 +783,7 @@
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="0.0000_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -805,10 +805,24 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7" tint="-0.25"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -955,7 +969,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -988,7 +1002,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1382,58 +1408,52 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1445,74 +1465,80 @@
     <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1576,19 +1602,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1941,18 +1988,18 @@
   <sheetPr/>
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="9" style="20"/>
     <col min="2" max="2" width="11.75" style="20" customWidth="1"/>
-    <col min="3" max="3" width="9" style="20"/>
-    <col min="4" max="4" width="12.625" style="20"/>
+    <col min="3" max="3" width="12.8916666666667" style="20"/>
+    <col min="4" max="4" width="12.6333333333333" style="20"/>
     <col min="5" max="5" width="9" style="20"/>
-    <col min="6" max="6" width="12.625" style="20"/>
+    <col min="6" max="6" width="12.6333333333333" style="20"/>
     <col min="7" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
@@ -1977,12 +2024,12 @@
       <c r="B2" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C2" s="20">
-        <v>5</v>
+      <c r="C2" s="30">
+        <v>4.80076812289966</v>
       </c>
       <c r="D2" s="20">
         <f>C2/1000/B2</f>
-        <v>0.0377358490566038</v>
+        <v>0.0362322122482993</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1992,12 +2039,12 @@
       <c r="B3" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C3" s="20">
-        <v>5</v>
+      <c r="C3" s="30">
+        <v>4.93339911198816</v>
       </c>
       <c r="D3" s="20">
         <f t="shared" ref="D3:D34" si="0">C3/1000/B3</f>
-        <v>0.0377358490566038</v>
+        <v>0.0372332008451937</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2007,12 +2054,12 @@
       <c r="B4" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C4" s="20">
-        <v>5</v>
+      <c r="C4" s="30">
+        <v>4.95908752789487</v>
       </c>
       <c r="D4" s="20">
         <f t="shared" si="0"/>
-        <v>0.0377358490566038</v>
+        <v>0.0374270756822254</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2022,12 +2069,12 @@
       <c r="B5" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C5" s="20">
-        <v>5</v>
+      <c r="C5" s="30">
+        <v>4.95908752789487</v>
       </c>
       <c r="D5" s="20">
         <f t="shared" si="0"/>
-        <v>0.0377358490566038</v>
+        <v>0.0374270756822254</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2037,12 +2084,12 @@
       <c r="B6" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C6" s="20">
-        <v>5</v>
+      <c r="C6" s="30">
+        <v>5.03651473180559</v>
       </c>
       <c r="D6" s="20">
         <f t="shared" si="0"/>
-        <v>0.0377358490566038</v>
+        <v>0.0380114319381554</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2052,12 +2099,12 @@
       <c r="B7" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C7" s="20">
-        <v>5</v>
+      <c r="C7" s="30">
+        <v>5.20020800832033</v>
       </c>
       <c r="D7" s="20">
         <f t="shared" si="0"/>
-        <v>0.0377358490566038</v>
+        <v>0.0392468528929836</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2067,12 +2114,12 @@
       <c r="B8" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C8" s="20">
-        <v>5</v>
+      <c r="C8" s="30">
+        <v>4.95908752789487</v>
       </c>
       <c r="D8" s="20">
         <f t="shared" si="0"/>
-        <v>0.0377358490566038</v>
+        <v>0.0374270756822254</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2082,12 +2129,12 @@
       <c r="B9" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C9" s="20">
-        <v>5</v>
+      <c r="C9" s="30">
+        <v>5.03651473180559</v>
       </c>
       <c r="D9" s="20">
         <f t="shared" si="0"/>
-        <v>0.0377358490566038</v>
+        <v>0.0380114319381554</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2097,12 +2144,12 @@
       <c r="B10" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C10" s="20">
-        <v>5</v>
+      <c r="C10" s="30">
+        <v>5.03651473180559</v>
       </c>
       <c r="D10" s="20">
         <f t="shared" si="0"/>
-        <v>0.0377358490566038</v>
+        <v>0.0380114319381554</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2112,12 +2159,12 @@
       <c r="B11" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C11" s="20">
-        <v>5</v>
+      <c r="C11" s="30">
+        <v>4.920049200492</v>
       </c>
       <c r="D11" s="20">
         <f t="shared" si="0"/>
-        <v>0.0377358490566038</v>
+        <v>0.037132446796166</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2127,12 +2174,12 @@
       <c r="B12" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C12" s="20">
-        <v>5</v>
+      <c r="C12" s="30">
+        <v>5.15862780500387</v>
       </c>
       <c r="D12" s="20">
         <f t="shared" si="0"/>
-        <v>0.0377358490566038</v>
+        <v>0.0389330400377651</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2142,12 +2189,12 @@
       <c r="B13" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C13" s="20">
-        <v>5</v>
+      <c r="C13" s="30">
+        <v>4.968944099</v>
       </c>
       <c r="D13" s="20">
         <f t="shared" si="0"/>
-        <v>0.0377358490566038</v>
+        <v>0.0375014648981132</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2157,12 +2204,12 @@
       <c r="B14" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C14" s="20">
-        <v>5</v>
+      <c r="C14" s="30">
+        <v>4.968944099</v>
       </c>
       <c r="D14" s="20">
         <f t="shared" si="0"/>
-        <v>0.0377358490566038</v>
+        <v>0.0375014648981132</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2172,12 +2219,12 @@
       <c r="B15" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C15" s="20">
-        <v>5</v>
+      <c r="C15" s="30">
+        <v>10.2564102564103</v>
       </c>
       <c r="D15" s="20">
         <f t="shared" si="0"/>
-        <v>0.0377358490566038</v>
+        <v>0.0774068698597004</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2187,12 +2234,12 @@
       <c r="B16" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C16" s="20">
-        <v>5</v>
+      <c r="C16" s="30">
+        <v>5.03651473180559</v>
       </c>
       <c r="D16" s="20">
         <f t="shared" si="0"/>
-        <v>0.0377358490566038</v>
+        <v>0.0380114319381554</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2202,12 +2249,12 @@
       <c r="B17" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C17" s="20">
-        <v>5</v>
+      <c r="C17" s="30">
+        <v>4.95908752789487</v>
       </c>
       <c r="D17" s="20">
         <f t="shared" si="0"/>
-        <v>0.0377358490566038</v>
+        <v>0.0374270756822254</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2217,12 +2264,12 @@
       <c r="B18" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C18" s="20">
-        <v>10</v>
+      <c r="C18" s="30">
+        <v>10.2933607822954</v>
       </c>
       <c r="D18" s="20">
         <f t="shared" si="0"/>
-        <v>0.0223015165031222</v>
+        <v>0.0229557555358952</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2232,12 +2279,12 @@
       <c r="B19" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C19" s="20">
-        <v>10</v>
+      <c r="C19" s="30">
+        <v>10.8166576527853</v>
       </c>
       <c r="D19" s="20">
         <f t="shared" si="0"/>
-        <v>0.0223015165031222</v>
+        <v>0.0241227869152215</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2247,12 +2294,12 @@
       <c r="B20" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C20" s="20">
-        <v>10</v>
+      <c r="C20" s="30">
+        <v>9.97506234413965</v>
       </c>
       <c r="D20" s="20">
         <f t="shared" si="0"/>
-        <v>0.0223015165031222</v>
+        <v>0.0222459017487503</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2262,12 +2309,12 @@
       <c r="B21" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C21" s="20">
-        <v>10</v>
+      <c r="C21" s="30">
+        <v>9.97506234413965</v>
       </c>
       <c r="D21" s="20">
         <f t="shared" si="0"/>
-        <v>0.0223015165031222</v>
+        <v>0.0222459017487503</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2277,12 +2324,12 @@
       <c r="B22" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C22" s="20">
-        <v>10</v>
+      <c r="C22" s="30">
+        <v>9.67117988394584</v>
       </c>
       <c r="D22" s="20">
         <f t="shared" si="0"/>
-        <v>0.0223015165031222</v>
+        <v>0.0215681977786482</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2292,12 +2339,12 @@
       <c r="B23" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C23" s="20">
-        <v>10</v>
+      <c r="C23" s="30">
+        <v>10.1317122593718</v>
       </c>
       <c r="D23" s="20">
         <f t="shared" si="0"/>
-        <v>0.0223015165031222</v>
+        <v>0.0225952548157266</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2307,12 +2354,12 @@
       <c r="B24" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C24" s="20">
-        <v>10</v>
+      <c r="C24" s="30">
+        <v>9.67117988394584</v>
       </c>
       <c r="D24" s="20">
         <f t="shared" si="0"/>
-        <v>0.0223015165031222</v>
+        <v>0.0215681977786482</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2322,12 +2369,12 @@
       <c r="B25" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C25" s="20">
-        <v>10</v>
+      <c r="C25" s="30">
+        <v>10.1317122593718</v>
       </c>
       <c r="D25" s="20">
         <f t="shared" si="0"/>
-        <v>0.0223015165031222</v>
+        <v>0.0225952548157266</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2337,12 +2384,12 @@
       <c r="B26" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C26" s="20">
-        <v>10</v>
+      <c r="C26" s="31">
+        <v>10.1317122593718</v>
       </c>
       <c r="D26" s="20">
         <f t="shared" si="0"/>
-        <v>0.0223015165031222</v>
+        <v>0.0225952548157266</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2352,12 +2399,12 @@
       <c r="B27" s="20">
         <v>0.335</v>
       </c>
-      <c r="C27" s="20">
-        <v>10</v>
+      <c r="C27" s="32">
+        <v>10.1317122593718</v>
       </c>
       <c r="D27" s="20">
         <f t="shared" si="0"/>
-        <v>0.0298507462686567</v>
+        <v>0.0302439171921546</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2368,11 +2415,11 @@
         <v>0.335</v>
       </c>
       <c r="C28" s="20">
-        <v>10</v>
+        <v>10.1255569056298</v>
       </c>
       <c r="D28" s="20">
         <f t="shared" si="0"/>
-        <v>0.0298507462686567</v>
+        <v>0.03022554300188</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2383,11 +2430,11 @@
         <v>0.335</v>
       </c>
       <c r="C29" s="20">
-        <v>10</v>
+        <v>10.1895251681272</v>
       </c>
       <c r="D29" s="20">
         <f t="shared" si="0"/>
-        <v>0.0298507462686567</v>
+        <v>0.0304164930391857</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2398,11 +2445,11 @@
         <v>0.335</v>
       </c>
       <c r="C30" s="20">
-        <v>10</v>
+        <v>10.0623867981485</v>
       </c>
       <c r="D30" s="20">
         <f t="shared" si="0"/>
-        <v>0.0298507462686567</v>
+        <v>0.0300369755168612</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2413,11 +2460,11 @@
         <v>0.335</v>
       </c>
       <c r="C31" s="20">
-        <v>10</v>
+        <v>10.0623867981485</v>
       </c>
       <c r="D31" s="20">
         <f t="shared" si="0"/>
-        <v>0.0298507462686567</v>
+        <v>0.0300369755168612</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2428,11 +2475,11 @@
         <v>0.335</v>
       </c>
       <c r="C32" s="20">
-        <v>10</v>
+        <v>9.93640699523053</v>
       </c>
       <c r="D32" s="20">
         <f t="shared" si="0"/>
-        <v>0.0298507462686567</v>
+        <v>0.0296609164036732</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2443,11 +2490,11 @@
         <v>0.335</v>
       </c>
       <c r="C33" s="20">
-        <v>10</v>
+        <v>10.2543068088597</v>
       </c>
       <c r="D33" s="20">
         <f t="shared" si="0"/>
-        <v>0.0298507462686567</v>
+        <v>0.030609871071223</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2458,11 +2505,11 @@
         <v>0.335</v>
       </c>
       <c r="C34" s="20">
-        <v>10</v>
+        <v>9.81546917942678</v>
       </c>
       <c r="D34" s="20">
         <f t="shared" si="0"/>
-        <v>0.0298507462686567</v>
+        <v>0.0292999079982889</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2473,11 +2520,11 @@
         <v>0.335</v>
       </c>
       <c r="C35" s="20">
-        <v>10</v>
+        <v>10.0623867981485</v>
       </c>
       <c r="D35" s="20">
         <f t="shared" ref="D35:D53" si="1">C35/1000/B35</f>
-        <v>0.0298507462686567</v>
+        <v>0.0300369755168612</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2488,11 +2535,11 @@
         <v>0.335</v>
       </c>
       <c r="C36" s="20">
-        <v>10</v>
+        <v>9.87556784515109</v>
       </c>
       <c r="D36" s="20">
         <f t="shared" si="1"/>
-        <v>0.0298507462686567</v>
+        <v>0.029479307000451</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2503,11 +2550,11 @@
         <v>0.335</v>
       </c>
       <c r="C37" s="20">
-        <v>10</v>
+        <v>10.1895251681272</v>
       </c>
       <c r="D37" s="20">
         <f t="shared" si="1"/>
-        <v>0.0298507462686567</v>
+        <v>0.0304164930391857</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2518,11 +2565,11 @@
         <v>0.335</v>
       </c>
       <c r="C38" s="20">
-        <v>10</v>
+        <v>9.99800039992001</v>
       </c>
       <c r="D38" s="20">
         <f t="shared" si="1"/>
-        <v>0.0298507462686567</v>
+        <v>0.0298447773131941</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2533,11 +2580,11 @@
         <v>0.335</v>
       </c>
       <c r="C39" s="20">
-        <v>10</v>
+        <v>9.87556784515109</v>
       </c>
       <c r="D39" s="20">
         <f t="shared" si="1"/>
-        <v>0.0298507462686567</v>
+        <v>0.029479307000451</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2548,11 +2595,11 @@
         <v>0.335</v>
       </c>
       <c r="C40" s="20">
-        <v>10</v>
+        <v>9.87556784515109</v>
       </c>
       <c r="D40" s="20">
         <f t="shared" si="1"/>
-        <v>0.0298507462686567</v>
+        <v>0.029479307000451</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2563,11 +2610,11 @@
         <v>0.335</v>
       </c>
       <c r="C41" s="20">
-        <v>10</v>
+        <v>9.99800039992001</v>
       </c>
       <c r="D41" s="20">
         <f t="shared" si="1"/>
-        <v>0.0298507462686567</v>
+        <v>0.0298447773131941</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2578,11 +2625,11 @@
         <v>0.335</v>
       </c>
       <c r="C42" s="20">
-        <v>10</v>
+        <v>10.1255569056298</v>
       </c>
       <c r="D42" s="20">
         <f t="shared" si="1"/>
-        <v>0.0298507462686567</v>
+        <v>0.03022554300188</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2593,11 +2640,11 @@
         <v>0.335</v>
       </c>
       <c r="C43" s="20">
-        <v>10</v>
+        <v>9.93640699523053</v>
       </c>
       <c r="D43" s="20">
         <f t="shared" si="1"/>
-        <v>0.0298507462686567</v>
+        <v>0.0296609164036732</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2608,11 +2655,11 @@
         <v>0.335</v>
       </c>
       <c r="C44" s="20">
-        <v>10</v>
+        <v>9.87556784515109</v>
       </c>
       <c r="D44" s="20">
         <f t="shared" si="1"/>
-        <v>0.0298507462686567</v>
+        <v>0.029479307000451</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2623,11 +2670,11 @@
         <v>0.4484</v>
       </c>
       <c r="C45" s="20">
-        <v>10</v>
+        <v>10.0623867981485</v>
       </c>
       <c r="D45" s="20">
         <f t="shared" si="1"/>
-        <v>0.0223015165031222</v>
+        <v>0.0224406485239708</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2638,11 +2685,11 @@
         <v>0.4484</v>
       </c>
       <c r="C46" s="20">
-        <v>10</v>
+        <v>10.2543068088597</v>
       </c>
       <c r="D46" s="20">
         <f t="shared" si="1"/>
-        <v>0.0223015165031222</v>
+        <v>0.0228686592525863</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2653,11 +2700,11 @@
         <v>0.4484</v>
       </c>
       <c r="C47" s="20">
-        <v>10</v>
+        <v>9.87556784515109</v>
       </c>
       <c r="D47" s="20">
         <f t="shared" si="1"/>
-        <v>0.0223015165031222</v>
+        <v>0.022024013927634</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2668,11 +2715,11 @@
         <v>0.4484</v>
       </c>
       <c r="C48" s="20">
-        <v>10</v>
+        <v>10.2543068088597</v>
       </c>
       <c r="D48" s="20">
         <f t="shared" si="1"/>
-        <v>0.0223015165031222</v>
+        <v>0.0228686592525863</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2683,11 +2730,11 @@
         <v>0.4484</v>
       </c>
       <c r="C49" s="20">
-        <v>10</v>
+        <v>9.87556784515109</v>
       </c>
       <c r="D49" s="20">
         <f t="shared" si="1"/>
-        <v>0.0223015165031222</v>
+        <v>0.022024013927634</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2698,11 +2745,11 @@
         <v>0.4484</v>
       </c>
       <c r="C50" s="20">
-        <v>10</v>
+        <v>10.078613182826</v>
       </c>
       <c r="D50" s="20">
         <f t="shared" si="1"/>
-        <v>0.0223015165031222</v>
+        <v>0.0224768358225379</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2713,11 +2760,11 @@
         <v>0.4484</v>
       </c>
       <c r="C51" s="20">
-        <v>10</v>
+        <v>9.89119683481701</v>
       </c>
       <c r="D51" s="20">
         <f t="shared" si="1"/>
-        <v>0.0223015165031222</v>
+        <v>0.0220588689447302</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2728,11 +2775,11 @@
         <v>0.4484</v>
       </c>
       <c r="C52" s="20">
-        <v>10</v>
+        <v>9.89119683481701</v>
       </c>
       <c r="D52" s="20">
         <f t="shared" si="1"/>
-        <v>0.0223015165031222</v>
+        <v>0.0220588689447302</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2743,11 +2790,11 @@
         <v>0.4484</v>
       </c>
       <c r="C53" s="20">
-        <v>10</v>
+        <v>10.4733975701718</v>
       </c>
       <c r="D53" s="20">
         <f t="shared" si="1"/>
-        <v>0.0223015165031222</v>
+        <v>0.0233572648754946</v>
       </c>
     </row>
   </sheetData>
@@ -2763,15 +2810,15 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="9" style="20"/>
-    <col min="2" max="2" width="12.125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="12.1333333333333" style="20" customWidth="1"/>
     <col min="3" max="3" width="9" style="20"/>
-    <col min="4" max="4" width="15.625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="15.6333333333333" style="20" customWidth="1"/>
     <col min="5" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
@@ -2797,11 +2844,11 @@
         <v>0.1</v>
       </c>
       <c r="C2" s="20">
-        <v>2</v>
+        <v>2.02839756592292</v>
       </c>
       <c r="D2" s="20">
         <f>C2/1000/B2</f>
-        <v>0.02</v>
+        <v>0.0202839756592292</v>
       </c>
     </row>
     <row r="3" s="20" customFormat="1" spans="1:4">
@@ -2812,11 +2859,11 @@
         <v>0.1</v>
       </c>
       <c r="C3" s="20">
-        <v>2</v>
+        <v>2.02839756592292</v>
       </c>
       <c r="D3" s="20">
         <f t="shared" ref="D3:D15" si="0">C3/1000/B3</f>
-        <v>0.02</v>
+        <v>0.0202839756592292</v>
       </c>
     </row>
     <row r="4" s="20" customFormat="1" spans="1:4">
@@ -2827,11 +2874,11 @@
         <v>0.1</v>
       </c>
       <c r="C4" s="20">
-        <v>2</v>
+        <v>2.02839756592292</v>
       </c>
       <c r="D4" s="20">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.0202839756592292</v>
       </c>
     </row>
     <row r="5" s="20" customFormat="1" spans="1:4">
@@ -2842,11 +2889,11 @@
         <v>0.1</v>
       </c>
       <c r="C5" s="20">
-        <v>2</v>
+        <v>2.02839756592292</v>
       </c>
       <c r="D5" s="20">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.0202839756592292</v>
       </c>
     </row>
     <row r="6" s="20" customFormat="1" spans="1:4">
@@ -2857,11 +2904,11 @@
         <v>0.1</v>
       </c>
       <c r="C6" s="20">
-        <v>2</v>
+        <v>2.02839756592292</v>
       </c>
       <c r="D6" s="20">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.0202839756592292</v>
       </c>
     </row>
     <row r="7" s="20" customFormat="1" spans="1:4">
@@ -2872,11 +2919,11 @@
         <v>0.1</v>
       </c>
       <c r="C7" s="20">
-        <v>2</v>
+        <v>2.04081632653061</v>
       </c>
       <c r="D7" s="20">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.0204081632653061</v>
       </c>
     </row>
     <row r="8" s="20" customFormat="1" spans="1:4">
@@ -2887,11 +2934,11 @@
         <v>0.1</v>
       </c>
       <c r="C8" s="20">
-        <v>2</v>
+        <v>2.02839756592292</v>
       </c>
       <c r="D8" s="20">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.0202839756592292</v>
       </c>
     </row>
     <row r="9" s="20" customFormat="1" spans="1:4">
@@ -2902,11 +2949,11 @@
         <v>0.1</v>
       </c>
       <c r="C9" s="20">
-        <v>2</v>
+        <v>2.04123290467442</v>
       </c>
       <c r="D9" s="20">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.0204123290467442</v>
       </c>
     </row>
     <row r="10" s="20" customFormat="1" spans="1:4">
@@ -2917,11 +2964,11 @@
         <v>0.1</v>
       </c>
       <c r="C10" s="20">
-        <v>2</v>
+        <v>2.04123290467442</v>
       </c>
       <c r="D10" s="20">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.0204123290467442</v>
       </c>
     </row>
     <row r="11" s="20" customFormat="1" spans="1:4">
@@ -2932,11 +2979,11 @@
         <v>0.1</v>
       </c>
       <c r="C11" s="20">
-        <v>2</v>
+        <v>2.02839756592292</v>
       </c>
       <c r="D11" s="20">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.0202839756592292</v>
       </c>
     </row>
     <row r="12" s="20" customFormat="1" spans="1:4">
@@ -2947,11 +2994,11 @@
         <v>0.1</v>
       </c>
       <c r="C12" s="20">
-        <v>2</v>
+        <v>2.02839756592292</v>
       </c>
       <c r="D12" s="20">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.0202839756592292</v>
       </c>
     </row>
     <row r="13" s="20" customFormat="1" spans="1:4">
@@ -2962,11 +3009,11 @@
         <v>0.1</v>
       </c>
       <c r="C13" s="20">
-        <v>2</v>
+        <v>2.04123290467442</v>
       </c>
       <c r="D13" s="20">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.0204123290467442</v>
       </c>
     </row>
     <row r="14" s="20" customFormat="1" spans="1:4">
@@ -2992,11 +3039,11 @@
         <v>0.2271</v>
       </c>
       <c r="C15" s="20">
-        <v>5</v>
+        <v>4.99900019996001</v>
       </c>
       <c r="D15" s="20">
         <f t="shared" si="0"/>
-        <v>0.0220167327168648</v>
+        <v>0.0220123302508147</v>
       </c>
     </row>
     <row r="16" s="20" customFormat="1" spans="1:4">
@@ -3007,11 +3054,11 @@
         <v>0.2271</v>
       </c>
       <c r="C16" s="20">
-        <v>5</v>
+        <v>4.99900019996001</v>
       </c>
       <c r="D16" s="20">
         <f t="shared" ref="D16:D49" si="1">C16/1000/B16</f>
-        <v>0.0220167327168648</v>
+        <v>0.0220123302508147</v>
       </c>
     </row>
     <row r="17" s="20" customFormat="1" spans="1:4">
@@ -3022,11 +3069,11 @@
         <v>0.2271</v>
       </c>
       <c r="C17" s="20">
-        <v>5</v>
+        <v>4.99900019996001</v>
       </c>
       <c r="D17" s="20">
         <f t="shared" si="1"/>
-        <v>0.0220167327168648</v>
+        <v>0.0220123302508147</v>
       </c>
     </row>
     <row r="18" s="20" customFormat="1" spans="1:4">
@@ -3037,11 +3084,11 @@
         <v>0.2271</v>
       </c>
       <c r="C18" s="20">
-        <v>5</v>
+        <v>4.99900019996001</v>
       </c>
       <c r="D18" s="20">
         <f t="shared" si="1"/>
-        <v>0.0220167327168648</v>
+        <v>0.0220123302508147</v>
       </c>
     </row>
     <row r="19" s="20" customFormat="1" spans="1:4">
@@ -3052,11 +3099,11 @@
         <v>0.2271</v>
       </c>
       <c r="C19" s="20">
-        <v>5</v>
+        <v>5.09476258406358</v>
       </c>
       <c r="D19" s="20">
         <f t="shared" si="1"/>
-        <v>0.0220167327168648</v>
+        <v>0.0224340052138423</v>
       </c>
     </row>
     <row r="20" s="20" customFormat="1" spans="1:4">
@@ -3067,11 +3114,11 @@
         <v>0.2271</v>
       </c>
       <c r="C20" s="20">
-        <v>5</v>
+        <v>4.96820349761526</v>
       </c>
       <c r="D20" s="20">
         <f t="shared" si="1"/>
-        <v>0.0220167327168648</v>
+        <v>0.0218767216979976</v>
       </c>
     </row>
     <row r="21" s="20" customFormat="1" spans="1:4">
@@ -3082,11 +3129,11 @@
         <v>0.2271</v>
       </c>
       <c r="C21" s="20">
-        <v>5</v>
+        <v>5.09476258406358</v>
       </c>
       <c r="D21" s="20">
         <f t="shared" si="1"/>
-        <v>0.0220167327168648</v>
+        <v>0.0224340052138423</v>
       </c>
     </row>
     <row r="22" s="20" customFormat="1" spans="1:4">
@@ -3097,416 +3144,416 @@
         <v>0.2271</v>
       </c>
       <c r="C22" s="20">
-        <v>5</v>
+        <v>4.93778392257555</v>
       </c>
       <c r="D22" s="20">
         <f t="shared" si="1"/>
-        <v>0.0220167327168648</v>
+        <v>0.0217427737673956</v>
       </c>
     </row>
     <row r="23" s="20" customFormat="1" spans="1:4">
       <c r="A23" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="25">
+      <c r="B23" s="28">
         <v>0.726</v>
       </c>
       <c r="C23" s="20">
-        <v>10</v>
+        <v>10.0623867981485</v>
       </c>
       <c r="D23" s="20">
         <f t="shared" si="1"/>
-        <v>0.0137741046831956</v>
+        <v>0.0138600369120503</v>
       </c>
     </row>
     <row r="24" s="20" customFormat="1" spans="1:4">
       <c r="A24" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="25">
+      <c r="B24" s="28">
         <v>0.726</v>
       </c>
       <c r="C24" s="20">
-        <v>10</v>
+        <v>10.0623867981485</v>
       </c>
       <c r="D24" s="20">
         <f t="shared" si="1"/>
-        <v>0.0137741046831956</v>
+        <v>0.0138600369120503</v>
       </c>
     </row>
     <row r="25" s="20" customFormat="1" spans="1:4">
       <c r="A25" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="25">
+      <c r="B25" s="28">
         <v>0.726</v>
       </c>
       <c r="C25" s="20">
-        <v>10</v>
+        <v>10.0623867981485</v>
       </c>
       <c r="D25" s="20">
         <f t="shared" si="1"/>
-        <v>0.0137741046831956</v>
+        <v>0.0138600369120503</v>
       </c>
     </row>
     <row r="26" s="20" customFormat="1" spans="1:4">
       <c r="A26" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="25">
+      <c r="B26" s="28">
         <v>0.726</v>
       </c>
       <c r="C26" s="20">
-        <v>5</v>
+        <v>4.96820349761526</v>
       </c>
       <c r="D26" s="20">
         <f t="shared" si="1"/>
-        <v>0.0068870523415978</v>
+        <v>0.00684325550635711</v>
       </c>
     </row>
     <row r="27" s="20" customFormat="1" spans="1:4">
       <c r="A27" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="25">
+      <c r="B27" s="28">
         <v>0.726</v>
       </c>
       <c r="C27" s="20">
-        <v>5</v>
+        <v>4.96820349761526</v>
       </c>
       <c r="D27" s="20">
         <f t="shared" si="1"/>
-        <v>0.0068870523415978</v>
+        <v>0.00684325550635711</v>
       </c>
     </row>
     <row r="28" s="20" customFormat="1" spans="1:4">
       <c r="A28" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="25">
+      <c r="B28" s="28">
         <v>0.726</v>
       </c>
       <c r="C28" s="20">
-        <v>5</v>
+        <v>4.96820349761526</v>
       </c>
       <c r="D28" s="20">
         <f t="shared" si="1"/>
-        <v>0.0068870523415978</v>
+        <v>0.00684325550635711</v>
       </c>
     </row>
     <row r="29" s="20" customFormat="1" spans="1:4">
       <c r="A29" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="25">
+      <c r="B29" s="28">
         <v>0.726</v>
       </c>
       <c r="C29" s="20">
-        <v>5</v>
+        <v>5.06277845281491</v>
       </c>
       <c r="D29" s="20">
         <f t="shared" si="1"/>
-        <v>0.0068870523415978</v>
+        <v>0.00697352403968996</v>
       </c>
     </row>
     <row r="30" s="20" customFormat="1" spans="1:4">
       <c r="A30" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="25">
+      <c r="B30" s="28">
         <v>0.726</v>
       </c>
       <c r="C30" s="20">
-        <v>5</v>
+        <v>4.93778392257555</v>
       </c>
       <c r="D30" s="20">
         <f t="shared" si="1"/>
-        <v>0.0068870523415978</v>
+        <v>0.00680135526525558</v>
       </c>
     </row>
     <row r="31" s="20" customFormat="1" spans="1:4">
       <c r="A31" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="25">
+      <c r="B31" s="28">
         <v>0.726</v>
       </c>
       <c r="C31" s="20">
-        <v>5</v>
+        <v>5.09476258406358</v>
       </c>
       <c r="D31" s="20">
         <f t="shared" si="1"/>
-        <v>0.0068870523415978</v>
+        <v>0.00701757931689198</v>
       </c>
     </row>
     <row r="32" s="20" customFormat="1" spans="1:4">
       <c r="A32" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="B32" s="25">
+      <c r="B32" s="28">
         <v>0.726</v>
       </c>
       <c r="C32" s="20">
-        <v>5</v>
+        <v>5.06277845281491</v>
       </c>
       <c r="D32" s="20">
         <f t="shared" si="1"/>
-        <v>0.0068870523415978</v>
+        <v>0.00697352403968996</v>
       </c>
     </row>
     <row r="33" s="20" customFormat="1" spans="1:4">
       <c r="A33" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B33" s="25">
+      <c r="B33" s="28">
         <v>0.726</v>
       </c>
       <c r="C33" s="20">
-        <v>5</v>
+        <v>5.15995872033024</v>
       </c>
       <c r="D33" s="20">
         <f t="shared" si="1"/>
-        <v>0.0068870523415978</v>
+        <v>0.00710738115747967</v>
       </c>
     </row>
     <row r="34" s="20" customFormat="1" spans="1:4">
       <c r="A34" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B34" s="25">
+      <c r="B34" s="28">
         <v>0.726</v>
       </c>
       <c r="C34" s="20">
-        <v>5</v>
+        <v>5.0709939148073</v>
       </c>
       <c r="D34" s="20">
         <f>-C34/1000/B34</f>
-        <v>-0.0068870523415978</v>
+        <v>-0.00698484010304036</v>
       </c>
     </row>
     <row r="35" s="20" customFormat="1" spans="1:4">
       <c r="A35" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B35" s="25">
+      <c r="B35" s="28">
         <v>0.726</v>
       </c>
       <c r="C35" s="20">
-        <v>5</v>
+        <v>5.0709939148073</v>
       </c>
       <c r="D35" s="20">
         <f>-C35/1000/B35</f>
-        <v>-0.0068870523415978</v>
+        <v>-0.00698484010304036</v>
       </c>
     </row>
     <row r="36" s="20" customFormat="1" spans="1:4">
       <c r="A36" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="25">
+      <c r="B36" s="28">
         <v>0.726</v>
       </c>
       <c r="C36" s="20">
-        <v>5</v>
+        <v>5.03930659141302</v>
       </c>
       <c r="D36" s="20">
         <f>-C36/1000/B36</f>
-        <v>-0.0068870523415978</v>
+        <v>-0.00694119365208405</v>
       </c>
     </row>
     <row r="37" s="20" customFormat="1" spans="1:4">
       <c r="A37" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B37" s="25">
+      <c r="B37" s="28">
         <v>0.726</v>
       </c>
       <c r="C37" s="20">
-        <v>5</v>
+        <v>5.03930659141302</v>
       </c>
       <c r="D37" s="20">
         <f>-C37/1000/B37</f>
-        <v>-0.0068870523415978</v>
+        <v>-0.00694119365208405</v>
       </c>
     </row>
     <row r="38" s="20" customFormat="1" spans="1:4">
       <c r="A38" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="B38" s="25">
+      <c r="B38" s="28">
         <v>0.726</v>
       </c>
-      <c r="C38" s="20">
-        <v>10</v>
+      <c r="C38" s="29">
+        <v>9.71345313258863</v>
       </c>
       <c r="D38" s="20">
         <f t="shared" si="1"/>
-        <v>0.0137741046831956</v>
+        <v>0.013379412028359</v>
       </c>
     </row>
     <row r="39" s="20" customFormat="1" spans="1:4">
       <c r="A39" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B39" s="25">
+      <c r="B39" s="28">
         <v>0.726</v>
       </c>
-      <c r="C39" s="20">
-        <v>10</v>
+      <c r="C39" s="29">
+        <v>10.1729399796541</v>
       </c>
       <c r="D39" s="20">
         <f t="shared" si="1"/>
-        <v>0.0137741046831956</v>
+        <v>0.0140123140215621</v>
       </c>
     </row>
     <row r="40" s="20" customFormat="1" spans="1:4">
       <c r="A40" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B40" s="25">
+      <c r="B40" s="28">
         <v>0.726</v>
       </c>
-      <c r="C40" s="20">
-        <v>10</v>
+      <c r="C40" s="29">
+        <v>10.1729399796541</v>
       </c>
       <c r="D40" s="20">
         <f t="shared" si="1"/>
-        <v>0.0137741046831956</v>
+        <v>0.0140123140215621</v>
       </c>
     </row>
     <row r="41" s="20" customFormat="1" spans="1:4">
       <c r="A41" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B41" s="25">
+      <c r="B41" s="28">
         <v>0.2271</v>
       </c>
       <c r="C41" s="20">
-        <v>5</v>
+        <v>5.0709939148073</v>
       </c>
       <c r="D41" s="20">
         <f t="shared" ref="D41:D49" si="2">-C41/1000/B41</f>
-        <v>-0.0220167327168648</v>
+        <v>-0.0223293435262321</v>
       </c>
     </row>
     <row r="42" s="20" customFormat="1" spans="1:4">
       <c r="A42" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="25">
+      <c r="B42" s="28">
         <v>0.2271</v>
       </c>
       <c r="C42" s="20">
-        <v>5</v>
+        <v>5.0709939148073</v>
       </c>
       <c r="D42" s="20">
         <f t="shared" si="2"/>
-        <v>-0.0220167327168648</v>
+        <v>-0.0223293435262321</v>
       </c>
     </row>
     <row r="43" s="20" customFormat="1" spans="1:4">
       <c r="A43" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B43" s="25">
+      <c r="B43" s="28">
         <v>0.2271</v>
       </c>
       <c r="C43" s="20">
-        <v>5</v>
+        <v>5.0709939148073</v>
       </c>
       <c r="D43" s="20">
         <f t="shared" si="2"/>
-        <v>-0.0220167327168648</v>
+        <v>-0.0223293435262321</v>
       </c>
     </row>
     <row r="44" s="20" customFormat="1" spans="1:4">
       <c r="A44" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B44" s="25">
+      <c r="B44" s="28">
         <v>0.2271</v>
       </c>
       <c r="C44" s="20">
-        <v>5</v>
+        <v>5.0709939148073</v>
       </c>
       <c r="D44" s="20">
         <f t="shared" si="2"/>
-        <v>-0.0220167327168648</v>
+        <v>-0.0223293435262321</v>
       </c>
     </row>
     <row r="45" s="20" customFormat="1" spans="1:4">
       <c r="A45" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B45" s="25">
+      <c r="B45" s="28">
         <v>0.2271</v>
       </c>
       <c r="C45" s="20">
-        <v>5</v>
+        <v>5.0709939148073</v>
       </c>
       <c r="D45" s="20">
         <f t="shared" si="2"/>
-        <v>-0.0220167327168648</v>
+        <v>-0.0223293435262321</v>
       </c>
     </row>
     <row r="46" s="20" customFormat="1" spans="1:4">
       <c r="A46" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B46" s="25">
+      <c r="B46" s="28">
         <v>0.2271</v>
       </c>
       <c r="C46" s="20">
-        <v>5</v>
+        <v>5.0709939148073</v>
       </c>
       <c r="D46" s="20">
         <f t="shared" si="2"/>
-        <v>-0.0220167327168648</v>
+        <v>-0.0223293435262321</v>
       </c>
     </row>
     <row r="47" s="20" customFormat="1" spans="1:4">
       <c r="A47" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="B47" s="25">
+      <c r="B47" s="28">
         <v>0.2271</v>
       </c>
       <c r="C47" s="20">
-        <v>5</v>
+        <v>5.0709939148073</v>
       </c>
       <c r="D47" s="20">
         <f t="shared" si="2"/>
-        <v>-0.0220167327168648</v>
+        <v>-0.0223293435262321</v>
       </c>
     </row>
     <row r="48" s="20" customFormat="1" spans="1:4">
       <c r="A48" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="B48" s="25">
+      <c r="B48" s="28">
         <v>0.2271</v>
       </c>
       <c r="C48" s="20">
-        <v>5</v>
+        <v>5.03930659141302</v>
       </c>
       <c r="D48" s="20">
         <f t="shared" si="2"/>
-        <v>-0.0220167327168648</v>
+        <v>-0.0221898132602951</v>
       </c>
     </row>
     <row r="49" s="20" customFormat="1" spans="1:4">
       <c r="A49" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="25">
+      <c r="B49" s="28">
         <v>0.2271</v>
       </c>
       <c r="C49" s="20">
-        <v>5</v>
+        <v>5.0709939148073</v>
       </c>
       <c r="D49" s="20">
         <f t="shared" si="2"/>
-        <v>-0.0220167327168648</v>
+        <v>-0.0223293435262321</v>
       </c>
     </row>
   </sheetData>
@@ -3522,19 +3569,19 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="20" customWidth="1"/>
-    <col min="2" max="2" width="11.375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="9" style="20"/>
-    <col min="5" max="5" width="8.625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="13.3833333333333" style="20" customWidth="1"/>
+    <col min="2" max="2" width="11.3833333333333" style="20" customWidth="1"/>
+    <col min="3" max="3" width="11.1333333333333" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9.44166666666667" style="20"/>
+    <col min="5" max="5" width="8.63333333333333" style="20" customWidth="1"/>
     <col min="6" max="6" width="9" style="20"/>
-    <col min="7" max="7" width="12.375" style="20" customWidth="1"/>
-    <col min="8" max="8" width="13.75" style="20"/>
+    <col min="7" max="7" width="12.3833333333333" style="20" customWidth="1"/>
+    <col min="8" max="8" width="14.1083333333333" style="20"/>
     <col min="9" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
@@ -3554,15 +3601,22 @@
         <v>106</v>
       </c>
       <c r="B2" s="20">
-        <v>510</v>
+        <v>500.951808436029</v>
       </c>
       <c r="C2" s="20">
-        <v>-0.085</v>
+        <v>-0.0834919680726715</v>
+      </c>
+      <c r="D2" s="21">
+        <v>500.951808436029</v>
+      </c>
+      <c r="E2" s="22">
+        <f>D2/1000/6</f>
+        <v>0.0834919680726715</v>
       </c>
       <c r="F2" s="20">
         <v>-0.085</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="23">
         <v>1.05141289587297</v>
       </c>
     </row>
@@ -3571,15 +3625,22 @@
         <v>107</v>
       </c>
       <c r="B3" s="20">
-        <v>510</v>
+        <v>508.854060655404</v>
       </c>
       <c r="C3" s="20">
-        <v>0.085</v>
+        <v>0.084809010109234</v>
+      </c>
+      <c r="D3" s="21">
+        <v>508.854060655404</v>
+      </c>
+      <c r="E3" s="22">
+        <f t="shared" ref="E3:E20" si="0">D3/1000/6</f>
+        <v>0.084809010109234</v>
       </c>
       <c r="F3" s="20">
         <v>0.085</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="23">
         <v>1.04497421034587</v>
       </c>
     </row>
@@ -3588,15 +3649,22 @@
         <v>108</v>
       </c>
       <c r="B4" s="20">
-        <v>510</v>
+        <v>508.854060655404</v>
       </c>
       <c r="C4" s="20">
-        <v>0.085</v>
+        <v>0.084809010109234</v>
+      </c>
+      <c r="D4" s="21">
+        <v>508.854060655404</v>
+      </c>
+      <c r="E4" s="22">
+        <f t="shared" si="0"/>
+        <v>0.084809010109234</v>
       </c>
       <c r="F4" s="20">
         <v>0.085</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="23">
         <v>1.02510720127584</v>
       </c>
     </row>
@@ -3605,15 +3673,22 @@
         <v>109</v>
       </c>
       <c r="B5" s="20">
-        <v>510</v>
+        <v>507.150826655847</v>
       </c>
       <c r="C5" s="20">
-        <v>0.085</v>
+        <v>0.0845251377759745</v>
+      </c>
+      <c r="D5" s="21">
+        <v>507.150826655847</v>
+      </c>
+      <c r="E5" s="22">
+        <f t="shared" si="0"/>
+        <v>0.0845251377759745</v>
       </c>
       <c r="F5" s="20">
         <v>0.085</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="23">
         <v>0.985542533840889</v>
       </c>
     </row>
@@ -3622,15 +3697,22 @@
         <v>110</v>
       </c>
       <c r="B6" s="20">
-        <v>510</v>
+        <v>494.559841740851</v>
       </c>
       <c r="C6" s="20">
-        <v>-0.085</v>
+        <v>-0.0824266402901418</v>
+      </c>
+      <c r="D6" s="21">
+        <v>494.559841740851</v>
+      </c>
+      <c r="E6" s="22">
+        <f t="shared" si="0"/>
+        <v>0.0824266402901418</v>
       </c>
       <c r="F6" s="20">
         <v>-0.085</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="23">
         <v>1.00790267040447</v>
       </c>
     </row>
@@ -3639,15 +3721,22 @@
         <v>111</v>
       </c>
       <c r="B7" s="20">
-        <v>510</v>
+        <v>503.981453482512</v>
       </c>
       <c r="C7" s="20">
-        <v>-0.085</v>
+        <v>-0.083996908913752</v>
+      </c>
+      <c r="D7" s="21">
+        <v>503.981453482512</v>
+      </c>
+      <c r="E7" s="22">
+        <f t="shared" si="0"/>
+        <v>0.083996908913752</v>
       </c>
       <c r="F7" s="20">
         <v>-0.085</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="23">
         <v>0.96769087183098</v>
       </c>
     </row>
@@ -3656,15 +3745,22 @@
         <v>112</v>
       </c>
       <c r="B8" s="20">
-        <v>510</v>
+        <v>477.099236641221</v>
       </c>
       <c r="C8" s="20">
-        <v>-0.085</v>
+        <v>-0.0795165394402035</v>
+      </c>
+      <c r="D8" s="21">
+        <v>477.099236641221</v>
+      </c>
+      <c r="E8" s="22">
+        <f t="shared" si="0"/>
+        <v>0.0795165394402035</v>
       </c>
       <c r="F8" s="20">
         <v>-0.085</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="23">
         <v>1.03246933791451</v>
       </c>
     </row>
@@ -3673,15 +3769,22 @@
         <v>113</v>
       </c>
       <c r="B9" s="20">
-        <v>510</v>
+        <v>503.981453482512</v>
       </c>
       <c r="C9" s="20">
-        <v>0.085</v>
+        <v>0.083996908913752</v>
+      </c>
+      <c r="D9" s="21">
+        <v>503.981453482512</v>
+      </c>
+      <c r="E9" s="22">
+        <f t="shared" si="0"/>
+        <v>0.083996908913752</v>
       </c>
       <c r="F9" s="20">
         <v>0.085</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="23">
         <v>1.03552235408932</v>
       </c>
     </row>
@@ -3690,15 +3793,22 @@
         <v>114</v>
       </c>
       <c r="B10" s="20">
-        <v>510</v>
+        <v>503.981453482512</v>
       </c>
       <c r="C10" s="20">
-        <v>-0.085</v>
+        <v>-0.083996908913752</v>
+      </c>
+      <c r="D10" s="21">
+        <v>503.981453482512</v>
+      </c>
+      <c r="E10" s="22">
+        <f t="shared" si="0"/>
+        <v>0.083996908913752</v>
       </c>
       <c r="F10" s="20">
         <v>-0.085</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="24">
         <v>1.30718497829121</v>
       </c>
     </row>
@@ -3707,15 +3817,22 @@
         <v>115</v>
       </c>
       <c r="B11" s="20">
-        <v>510</v>
+        <v>491.642084562439</v>
       </c>
       <c r="C11" s="20">
-        <v>-0.085</v>
+        <v>-0.0819403474270732</v>
+      </c>
+      <c r="D11" s="21">
+        <v>491.642084562439</v>
+      </c>
+      <c r="E11" s="22">
+        <f t="shared" si="0"/>
+        <v>0.0819403474270732</v>
       </c>
       <c r="F11" s="20">
         <v>-0.085</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="24">
         <v>1.58590805403929</v>
       </c>
     </row>
@@ -3724,15 +3841,22 @@
         <v>116</v>
       </c>
       <c r="B12" s="20">
-        <v>510</v>
+        <v>494.559841740851</v>
       </c>
       <c r="C12" s="20">
-        <v>-0.085</v>
+        <v>-0.0824266402901418</v>
+      </c>
+      <c r="D12" s="21">
+        <v>494.559841740851</v>
+      </c>
+      <c r="E12" s="22">
+        <f t="shared" si="0"/>
+        <v>0.0824266402901418</v>
       </c>
       <c r="F12" s="20">
         <v>-0.085</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="24">
         <v>1.16091508958913</v>
       </c>
     </row>
@@ -3741,15 +3865,22 @@
         <v>117</v>
       </c>
       <c r="B13" s="20">
-        <v>510</v>
+        <v>503.981453482512</v>
       </c>
       <c r="C13" s="20">
-        <v>-0.085</v>
+        <v>-0.083996908913752</v>
+      </c>
+      <c r="D13" s="21">
+        <v>503.981453482512</v>
+      </c>
+      <c r="E13" s="22">
+        <f t="shared" si="0"/>
+        <v>0.083996908913752</v>
       </c>
       <c r="F13" s="20">
         <v>-0.085</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="23">
         <v>0.999311540469612</v>
       </c>
     </row>
@@ -3758,15 +3889,22 @@
         <v>118</v>
       </c>
       <c r="B14" s="20">
-        <v>510</v>
+        <v>513.663447709061</v>
       </c>
       <c r="C14" s="20">
-        <v>0.085</v>
+        <v>0.0856105746181768</v>
+      </c>
+      <c r="D14" s="21">
+        <v>513.663447709061</v>
+      </c>
+      <c r="E14" s="22">
+        <f t="shared" si="0"/>
+        <v>0.0856105746181768</v>
       </c>
       <c r="F14" s="20">
         <v>0.085</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="23">
         <v>0.954487879262718</v>
       </c>
     </row>
@@ -3775,15 +3913,22 @@
         <v>119</v>
       </c>
       <c r="B15" s="20">
-        <v>510</v>
+        <v>503.981453482512</v>
       </c>
       <c r="C15" s="20">
-        <v>-0.085</v>
+        <v>-0.083996908913752</v>
+      </c>
+      <c r="D15" s="21">
+        <v>503.981453482512</v>
+      </c>
+      <c r="E15" s="22">
+        <f t="shared" si="0"/>
+        <v>0.083996908913752</v>
       </c>
       <c r="F15" s="20">
         <v>-0.085</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="23">
         <v>0.982295081018815</v>
       </c>
     </row>
@@ -3792,15 +3937,22 @@
         <v>120</v>
       </c>
       <c r="B16" s="20">
-        <v>510</v>
+        <v>513.663447709061</v>
       </c>
       <c r="C16" s="20">
-        <v>0.085</v>
+        <v>0.0856105746181768</v>
+      </c>
+      <c r="D16" s="21">
+        <v>513.663447709061</v>
+      </c>
+      <c r="E16" s="22">
+        <f t="shared" si="0"/>
+        <v>0.0856105746181768</v>
       </c>
       <c r="F16" s="20">
         <v>0.085</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="23">
         <v>0.97702070710649</v>
       </c>
     </row>
@@ -3809,15 +3961,22 @@
         <v>121</v>
       </c>
       <c r="B17" s="20">
-        <v>510</v>
+        <v>513.663447709061</v>
       </c>
       <c r="C17" s="20">
-        <v>0.085</v>
+        <v>0.0856105746181768</v>
+      </c>
+      <c r="D17" s="21">
+        <v>513.663447709061</v>
+      </c>
+      <c r="E17" s="22">
+        <f t="shared" si="0"/>
+        <v>0.0856105746181768</v>
       </c>
       <c r="F17" s="20">
         <v>0.085</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="23">
         <v>0.9479618744931</v>
       </c>
     </row>
@@ -3826,15 +3985,22 @@
         <v>122</v>
       </c>
       <c r="B18" s="20">
-        <v>510</v>
+        <v>503.981453482512</v>
       </c>
       <c r="C18" s="20">
-        <v>-0.085</v>
+        <v>-0.083996908913752</v>
+      </c>
+      <c r="D18" s="21">
+        <v>503.981453482512</v>
+      </c>
+      <c r="E18" s="22">
+        <f t="shared" si="0"/>
+        <v>0.083996908913752</v>
       </c>
       <c r="F18" s="20">
         <v>-0.085</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="23">
         <v>0.792927641006873</v>
       </c>
     </row>
@@ -3843,15 +4009,22 @@
         <v>123</v>
       </c>
       <c r="B19" s="20">
-        <v>510</v>
+        <v>510.41241322989</v>
       </c>
       <c r="C19" s="20">
-        <v>0.085</v>
+        <v>0.085068735538315</v>
+      </c>
+      <c r="D19" s="21">
+        <v>510.41241322989</v>
+      </c>
+      <c r="E19" s="22">
+        <f t="shared" si="0"/>
+        <v>0.085068735538315</v>
       </c>
       <c r="F19" s="20">
         <v>0.085</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="23">
         <v>0.936397974673713</v>
       </c>
     </row>
@@ -3860,15 +4033,22 @@
         <v>124</v>
       </c>
       <c r="B20" s="20">
-        <v>510</v>
+        <v>494.559841740851</v>
       </c>
       <c r="C20" s="20">
-        <v>-0.085</v>
+        <v>-0.0824266402901418</v>
+      </c>
+      <c r="D20" s="21">
+        <v>494.559841740851</v>
+      </c>
+      <c r="E20" s="22">
+        <f t="shared" si="0"/>
+        <v>0.0824266402901418</v>
       </c>
       <c r="F20" s="20">
         <v>-0.085</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G20" s="23">
         <v>0.984456916873171</v>
       </c>
     </row>
@@ -3877,15 +4057,16 @@
         <v>125</v>
       </c>
       <c r="B21" s="20">
-        <v>100</v>
+        <v>98.9119683481701</v>
       </c>
       <c r="C21" s="20">
-        <v>-0.1</v>
+        <f>-B21/1000</f>
+        <v>-0.0989119683481701</v>
       </c>
       <c r="F21" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="23">
         <v>0.963505342010869</v>
       </c>
     </row>
@@ -3894,15 +4075,16 @@
         <v>126</v>
       </c>
       <c r="B22" s="20">
-        <v>100</v>
+        <v>99.5024875621891</v>
       </c>
       <c r="C22" s="20">
-        <v>-0.1</v>
+        <f t="shared" ref="C22:C30" si="1">-B22/1000</f>
+        <v>-0.0995024875621891</v>
       </c>
       <c r="F22" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G22" s="21">
+      <c r="G22" s="23">
         <v>0.954644492227053</v>
       </c>
     </row>
@@ -3911,15 +4093,16 @@
         <v>127</v>
       </c>
       <c r="B23" s="20">
-        <v>100</v>
+        <v>98.9119683481701</v>
       </c>
       <c r="C23" s="20">
-        <v>-0.1</v>
+        <f t="shared" si="1"/>
+        <v>-0.0989119683481701</v>
       </c>
       <c r="F23" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G23" s="23">
         <v>0.987926729944811</v>
       </c>
     </row>
@@ -3928,15 +4111,16 @@
         <v>128</v>
       </c>
       <c r="B24" s="20">
-        <v>100</v>
+        <v>98.9119683481701</v>
       </c>
       <c r="C24" s="20">
-        <v>-0.1</v>
+        <f t="shared" si="1"/>
+        <v>-0.0989119683481701</v>
       </c>
       <c r="F24" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G24" s="21">
+      <c r="G24" s="23">
         <v>1.0059675104667</v>
       </c>
     </row>
@@ -3945,15 +4129,16 @@
         <v>129</v>
       </c>
       <c r="B25" s="20">
-        <v>100</v>
+        <v>97.0873786407767</v>
       </c>
       <c r="C25" s="20">
-        <v>-0.1</v>
+        <f t="shared" si="1"/>
+        <v>-0.0970873786407767</v>
       </c>
       <c r="F25" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G25" s="21">
+      <c r="G25" s="23">
         <v>0.959971805022039</v>
       </c>
     </row>
@@ -3962,15 +4147,16 @@
         <v>130</v>
       </c>
       <c r="B26" s="20">
-        <v>100</v>
+        <v>98.9119683481701</v>
       </c>
       <c r="C26" s="20">
-        <v>-0.1</v>
+        <f t="shared" si="1"/>
+        <v>-0.0989119683481701</v>
       </c>
       <c r="F26" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G26" s="21">
+      <c r="G26" s="23">
         <v>0.967885395533345</v>
       </c>
     </row>
@@ -3979,15 +4165,16 @@
         <v>131</v>
       </c>
       <c r="B27" s="20">
-        <v>100</v>
+        <v>95.4198473282443</v>
       </c>
       <c r="C27" s="20">
-        <v>-0.1</v>
+        <f t="shared" si="1"/>
+        <v>-0.0954198473282443</v>
       </c>
       <c r="F27" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G27" s="21">
+      <c r="G27" s="23">
         <v>0.984344323774322</v>
       </c>
     </row>
@@ -3996,15 +4183,16 @@
         <v>132</v>
       </c>
       <c r="B28" s="20">
-        <v>100</v>
+        <v>100.796290696502</v>
       </c>
       <c r="C28" s="20">
-        <v>-0.1</v>
+        <f t="shared" si="1"/>
+        <v>-0.100796290696502</v>
       </c>
       <c r="F28" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G28" s="21">
+      <c r="G28" s="23">
         <v>0.954694884327784</v>
       </c>
     </row>
@@ -4013,15 +4201,16 @@
         <v>133</v>
       </c>
       <c r="B29" s="20">
-        <v>100</v>
+        <v>99.5024875621891</v>
       </c>
       <c r="C29" s="20">
-        <v>-0.1</v>
+        <f t="shared" si="1"/>
+        <v>-0.0995024875621891</v>
       </c>
       <c r="F29" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G29" s="21">
+      <c r="G29" s="23">
         <v>0.976404603726166</v>
       </c>
     </row>
@@ -4030,15 +4219,16 @@
         <v>134</v>
       </c>
       <c r="B30" s="20">
-        <v>100</v>
+        <v>97.0873786407767</v>
       </c>
       <c r="C30" s="20">
-        <v>-0.1</v>
+        <f t="shared" si="1"/>
+        <v>-0.0970873786407767</v>
       </c>
       <c r="F30" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G30" s="21">
+      <c r="G30" s="23">
         <v>0.991395400914359</v>
       </c>
     </row>
@@ -4047,15 +4237,16 @@
         <v>135</v>
       </c>
       <c r="B31" s="20">
-        <v>300</v>
+        <v>314.267756128221</v>
       </c>
       <c r="C31" s="20">
-        <v>-0.3</v>
+        <f t="shared" ref="C31:C48" si="2">-B31/1000</f>
+        <v>-0.314267756128221</v>
       </c>
       <c r="F31" s="20">
         <v>-0.3</v>
       </c>
-      <c r="G31" s="21">
+      <c r="G31" s="23">
         <v>0.965521196122588</v>
       </c>
     </row>
@@ -4064,86 +4255,91 @@
         <v>136</v>
       </c>
       <c r="B32" s="20">
-        <v>300</v>
+        <v>304.692260816575</v>
       </c>
       <c r="C32" s="20">
-        <v>-0.3</v>
+        <f t="shared" si="2"/>
+        <v>-0.304692260816575</v>
       </c>
       <c r="F32" s="20">
         <v>-0.3</v>
       </c>
-      <c r="G32" s="22">
+      <c r="G32" s="24">
         <v>2.03626250365614</v>
       </c>
     </row>
     <row r="33" ht="14.25" spans="1:7">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="25" t="s">
         <v>137</v>
       </c>
       <c r="B33" s="20">
-        <v>300</v>
+        <v>293.427230046948</v>
       </c>
       <c r="C33" s="20">
-        <v>-0.3</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>138</v>
+        <f t="shared" si="2"/>
+        <v>-0.293427230046948</v>
       </c>
       <c r="F33" s="20">
         <v>-0.3</v>
       </c>
-      <c r="G33" s="21">
+      <c r="G33" s="23">
         <v>0.992055264033481</v>
       </c>
     </row>
     <row r="34" ht="14.25" spans="1:7">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" s="26">
+        <v>296.73590504451</v>
+      </c>
+      <c r="C34" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.29673590504451</v>
+      </c>
+      <c r="D34" s="20" t="s">
         <v>139</v>
-      </c>
-      <c r="B34" s="24">
-        <v>300</v>
-      </c>
-      <c r="C34" s="20">
-        <v>-0.3</v>
       </c>
       <c r="F34" s="20">
         <v>-0.3</v>
       </c>
-      <c r="G34" s="21">
+      <c r="G34" s="23">
         <v>0.996409927774611</v>
       </c>
     </row>
     <row r="35" ht="14.25" spans="1:7">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="B35" s="24">
-        <v>300</v>
-      </c>
-      <c r="C35" s="20">
-        <v>0.3</v>
+      <c r="B35" s="26">
+        <v>296.73590504451</v>
+      </c>
+      <c r="C35" s="27">
+        <f t="shared" si="2"/>
+        <v>-0.29673590504451</v>
       </c>
       <c r="F35" s="20">
         <v>0.3</v>
       </c>
-      <c r="G35" s="21">
+      <c r="G35" s="23">
         <v>0.990366511511847</v>
       </c>
     </row>
     <row r="36" ht="14.25" spans="1:7">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="25" t="s">
         <v>141</v>
       </c>
       <c r="B36" s="20">
-        <v>300</v>
+        <v>293.427230046948</v>
       </c>
       <c r="C36" s="20">
-        <v>-0.3</v>
+        <f t="shared" si="2"/>
+        <v>-0.293427230046948</v>
       </c>
       <c r="F36" s="20">
         <v>-0.3</v>
       </c>
-      <c r="G36" s="21">
+      <c r="G36" s="23">
         <v>1.00101116548929</v>
       </c>
     </row>
@@ -4152,15 +4348,16 @@
         <v>142</v>
       </c>
       <c r="B37" s="20">
-        <v>300</v>
+        <v>285.225328009127</v>
       </c>
       <c r="C37" s="20">
-        <v>-0.3</v>
+        <f t="shared" si="2"/>
+        <v>-0.285225328009127</v>
       </c>
       <c r="F37" s="20">
         <v>-0.3</v>
       </c>
-      <c r="G37" s="21">
+      <c r="G37" s="23">
         <v>1.04690459254695</v>
       </c>
     </row>
@@ -4169,15 +4366,16 @@
         <v>143</v>
       </c>
       <c r="B38" s="20">
-        <v>300</v>
+        <v>314.267756128221</v>
       </c>
       <c r="C38" s="20">
-        <v>-0.3</v>
+        <f t="shared" si="2"/>
+        <v>-0.314267756128221</v>
       </c>
       <c r="F38" s="20">
         <v>-0.3</v>
       </c>
-      <c r="G38" s="21">
+      <c r="G38" s="23">
         <v>0.95124107406349</v>
       </c>
     </row>
@@ -4186,15 +4384,16 @@
         <v>144</v>
       </c>
       <c r="B39" s="20">
-        <v>100</v>
+        <v>100.78613182826</v>
       </c>
       <c r="C39" s="20">
-        <v>-0.1</v>
+        <f t="shared" si="2"/>
+        <v>-0.10078613182826</v>
       </c>
       <c r="F39" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G39" s="21">
+      <c r="G39" s="23">
         <v>0.786490532132579</v>
       </c>
     </row>
@@ -4203,15 +4402,16 @@
         <v>145</v>
       </c>
       <c r="B40" s="20">
-        <v>100</v>
+        <v>99.5421063109695</v>
       </c>
       <c r="C40" s="20">
-        <v>-0.1</v>
+        <f t="shared" si="2"/>
+        <v>-0.0995421063109695</v>
       </c>
       <c r="F40" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G40" s="21">
+      <c r="G40" s="23">
         <v>1.00513452816592</v>
       </c>
     </row>
@@ -4220,15 +4420,16 @@
         <v>146</v>
       </c>
       <c r="B41" s="20">
-        <v>100</v>
+        <v>98.9119683481701</v>
       </c>
       <c r="C41" s="20">
-        <v>-0.1</v>
+        <f t="shared" si="2"/>
+        <v>-0.0989119683481701</v>
       </c>
       <c r="F41" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G41" s="21">
+      <c r="G41" s="23">
         <v>1.0189075012981</v>
       </c>
     </row>
@@ -4237,15 +4438,16 @@
         <v>147</v>
       </c>
       <c r="B42" s="20">
-        <v>100</v>
+        <v>98.9119683481701</v>
       </c>
       <c r="C42" s="20">
-        <v>-0.1</v>
+        <f t="shared" si="2"/>
+        <v>-0.0989119683481701</v>
       </c>
       <c r="F42" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G42" s="21">
+      <c r="G42" s="23">
         <v>-0.00148210066326318</v>
       </c>
     </row>
@@ -4254,15 +4456,16 @@
         <v>148</v>
       </c>
       <c r="B43" s="20">
-        <v>100</v>
+        <v>98.9119683481701</v>
       </c>
       <c r="C43" s="20">
-        <v>-0.1</v>
+        <f t="shared" si="2"/>
+        <v>-0.0989119683481701</v>
       </c>
       <c r="F43" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G43" s="21">
+      <c r="G43" s="23">
         <v>1.04013828913163</v>
       </c>
     </row>
@@ -4271,15 +4474,16 @@
         <v>149</v>
       </c>
       <c r="B44" s="20">
-        <v>100</v>
+        <v>102.732689541812</v>
       </c>
       <c r="C44" s="20">
-        <v>-0.1</v>
+        <f t="shared" si="2"/>
+        <v>-0.102732689541812</v>
       </c>
       <c r="F44" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G44" s="21">
+      <c r="G44" s="23">
         <v>1.00120686910651</v>
       </c>
     </row>
@@ -4288,15 +4492,15 @@
         <v>150</v>
       </c>
       <c r="B45" s="20">
-        <v>100</v>
-      </c>
-      <c r="C45" s="20">
+        <v>98.9119683481701</v>
+      </c>
+      <c r="C45" s="27">
         <v>-0.1</v>
       </c>
       <c r="F45" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G45" s="21">
+      <c r="G45" s="23">
         <v>0.00585427974686723</v>
       </c>
     </row>
@@ -4305,15 +4509,16 @@
         <v>151</v>
       </c>
       <c r="B46" s="20">
-        <v>100</v>
+        <v>104.733975701718</v>
       </c>
       <c r="C46" s="20">
-        <v>-0.1</v>
+        <f>-B45/1000</f>
+        <v>-0.0989119683481701</v>
       </c>
       <c r="F46" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G46" s="21">
+      <c r="G46" s="23">
         <v>1.042062362991</v>
       </c>
     </row>
@@ -4322,15 +4527,16 @@
         <v>152</v>
       </c>
       <c r="B47" s="20">
-        <v>100</v>
+        <v>97.1250971250971</v>
       </c>
       <c r="C47" s="20">
-        <v>-0.1</v>
+        <f>-B46/1000</f>
+        <v>-0.104733975701718</v>
       </c>
       <c r="F47" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G47" s="21">
+      <c r="G47" s="23">
         <v>0.979760564664813</v>
       </c>
     </row>
@@ -4342,12 +4548,13 @@
         <v>100</v>
       </c>
       <c r="C48" s="20">
-        <v>-0.1</v>
+        <f>-B47/1000</f>
+        <v>-0.0971250971250971</v>
       </c>
       <c r="F48" s="20">
         <v>-0.1</v>
       </c>
-      <c r="G48" s="21">
+      <c r="G48" s="23">
         <v>1.0710899688599</v>
       </c>
     </row>
@@ -4367,16 +4574,16 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="25" customHeight="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="10.8833333333333" defaultRowHeight="25" customHeight="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="2" width="10.875" customWidth="1"/>
-    <col min="3" max="3" width="30.125" customWidth="1"/>
-    <col min="4" max="4" width="13.875" customWidth="1"/>
-    <col min="5" max="5" width="10.875" customWidth="1"/>
+    <col min="1" max="2" width="10.8833333333333" customWidth="1"/>
+    <col min="3" max="3" width="30.1333333333333" customWidth="1"/>
+    <col min="4" max="4" width="13.8833333333333" customWidth="1"/>
+    <col min="5" max="5" width="10.8833333333333" customWidth="1"/>
     <col min="6" max="6" width="18.75" customWidth="1"/>
-    <col min="7" max="7" width="14.4583333333333" customWidth="1"/>
-    <col min="8" max="8" width="17.125" customWidth="1"/>
-    <col min="9" max="16384" width="10.875" customWidth="1"/>
+    <col min="7" max="7" width="14.45" customWidth="1"/>
+    <col min="8" max="8" width="17.1333333333333" customWidth="1"/>
+    <col min="9" max="16384" width="10.8833333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:8">

</xml_diff>

<commit_message>
modify the parameter,manyshots etc
</commit_message>
<xml_diff>
--- a/diagnostics/emd/data/EXL50U coefficient.xlsx
+++ b/diagnostics/emd/data/EXL50U coefficient.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375" activeTab="2"/>
+    <workbookView windowWidth="27945" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="mpt" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="248">
   <si>
     <t>channel</t>
   </si>
@@ -44,6 +44,9 @@
     <t>K</t>
   </si>
   <si>
+    <t>方向标定（逆时针为正）</t>
+  </si>
+  <si>
     <t>MP001T</t>
   </si>
   <si>
@@ -200,6 +203,9 @@
     <t>MP052T</t>
   </si>
   <si>
+    <t>方向标定（向外为正）</t>
+  </si>
+  <si>
     <t>MP085n</t>
   </si>
   <si>
@@ -350,6 +356,9 @@
     <t>k</t>
   </si>
   <si>
+    <t>方向（PF正电流，输出为正）</t>
+  </si>
+  <si>
     <t>Flux001</t>
   </si>
   <si>
@@ -447,9 +456,6 @@
   </si>
   <si>
     <t>Flux033</t>
-  </si>
-  <si>
-    <t>环电压</t>
   </si>
   <si>
     <t>Flux034</t>
@@ -783,7 +789,7 @@
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="0.0000_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -807,16 +813,10 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="7" tint="-0.25"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -969,7 +969,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -997,12 +997,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB8CCE4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1408,52 +1402,55 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1468,77 +1465,74 @@
     <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1602,25 +1596,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1629,7 +1617,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1986,24 +1974,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="9" style="20"/>
     <col min="2" max="2" width="11.75" style="20" customWidth="1"/>
     <col min="3" max="3" width="12.8916666666667" style="20"/>
-    <col min="4" max="4" width="12.6333333333333" style="20"/>
+    <col min="4" max="4" width="13.75" style="20"/>
     <col min="5" max="5" width="9" style="20"/>
     <col min="6" max="6" width="12.6333333333333" style="20"/>
     <col min="7" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -2016,400 +2004,481 @@
       <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="28">
         <v>4.80076812289966</v>
       </c>
       <c r="D2" s="20">
-        <f>C2/1000/B2</f>
+        <f>C2/1000/B2*E2</f>
         <v>0.0362322122482993</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="28">
         <v>4.93339911198816</v>
       </c>
       <c r="D3" s="20">
-        <f t="shared" ref="D3:D34" si="0">C3/1000/B3</f>
+        <f t="shared" ref="D3:D34" si="0">C3/1000/B3*E3</f>
         <v>0.0372332008451937</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="28">
         <v>4.95908752789487</v>
       </c>
       <c r="D4" s="20">
         <f t="shared" si="0"/>
         <v>0.0374270756822254</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="28">
         <v>4.95908752789487</v>
       </c>
       <c r="D5" s="20">
         <f t="shared" si="0"/>
         <v>0.0374270756822254</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="28">
         <v>5.03651473180559</v>
       </c>
       <c r="D6" s="20">
         <f t="shared" si="0"/>
         <v>0.0380114319381554</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="28">
         <v>5.20020800832033</v>
       </c>
       <c r="D7" s="20">
         <f t="shared" si="0"/>
         <v>0.0392468528929836</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="28">
         <v>4.95908752789487</v>
       </c>
       <c r="D8" s="20">
         <f t="shared" si="0"/>
         <v>0.0374270756822254</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="28">
         <v>5.03651473180559</v>
       </c>
       <c r="D9" s="20">
         <f t="shared" si="0"/>
         <v>0.0380114319381554</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="28">
         <v>5.03651473180559</v>
       </c>
       <c r="D10" s="20">
         <f t="shared" si="0"/>
         <v>0.0380114319381554</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="28">
         <v>4.920049200492</v>
       </c>
       <c r="D11" s="20">
         <f t="shared" si="0"/>
         <v>0.037132446796166</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="28">
         <v>5.15862780500387</v>
       </c>
       <c r="D12" s="20">
         <f t="shared" si="0"/>
         <v>0.0389330400377651</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="28">
         <v>4.968944099</v>
       </c>
       <c r="D13" s="20">
         <f t="shared" si="0"/>
         <v>0.0375014648981132</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C14" s="30">
+      <c r="C14" s="28">
         <v>4.968944099</v>
       </c>
       <c r="D14" s="20">
         <f t="shared" si="0"/>
         <v>0.0375014648981132</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="28">
         <v>10.2564102564103</v>
       </c>
       <c r="D15" s="20">
         <f t="shared" si="0"/>
         <v>0.0774068698597004</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="28">
         <v>5.03651473180559</v>
       </c>
       <c r="D16" s="20">
         <f t="shared" si="0"/>
         <v>0.0380114319381554</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="20">
         <v>0.1325</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="28">
         <v>4.95908752789487</v>
       </c>
       <c r="D17" s="20">
         <f t="shared" si="0"/>
         <v>0.0374270756822254</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="28">
         <v>10.2933607822954</v>
       </c>
       <c r="D18" s="20">
         <f t="shared" si="0"/>
         <v>0.0229557555358952</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="28">
         <v>10.8166576527853</v>
       </c>
       <c r="D19" s="20">
         <f t="shared" si="0"/>
         <v>0.0241227869152215</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="28">
         <v>9.97506234413965</v>
       </c>
       <c r="D20" s="20">
         <f t="shared" si="0"/>
         <v>0.0222459017487503</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C21" s="30">
+      <c r="C21" s="28">
         <v>9.97506234413965</v>
       </c>
       <c r="D21" s="20">
         <f t="shared" si="0"/>
         <v>0.0222459017487503</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C22" s="30">
+      <c r="C22" s="28">
         <v>9.67117988394584</v>
       </c>
       <c r="D22" s="20">
         <f t="shared" si="0"/>
         <v>0.0215681977786482</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C23" s="30">
+      <c r="C23" s="28">
         <v>10.1317122593718</v>
       </c>
       <c r="D23" s="20">
         <f t="shared" si="0"/>
         <v>0.0225952548157266</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B24" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C24" s="30">
+      <c r="C24" s="28">
         <v>9.67117988394584</v>
       </c>
       <c r="D24" s="20">
         <f t="shared" si="0"/>
         <v>0.0215681977786482</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C25" s="30">
+      <c r="C25" s="28">
         <v>10.1317122593718</v>
       </c>
       <c r="D25" s="20">
         <f t="shared" si="0"/>
         <v>0.0225952548157266</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26" s="20">
         <v>0.4484</v>
       </c>
-      <c r="C26" s="31">
+      <c r="C26" s="29">
         <v>10.1317122593718</v>
       </c>
       <c r="D26" s="20">
         <f t="shared" si="0"/>
         <v>0.0225952548157266</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" s="20">
         <v>0.335</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="30">
         <v>10.1317122593718</v>
       </c>
       <c r="D27" s="20">
         <f t="shared" si="0"/>
-        <v>0.0302439171921546</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>-0.0302439171921546</v>
+      </c>
+      <c r="E27" s="20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28" s="20">
         <v>0.335</v>
@@ -2419,12 +2488,15 @@
       </c>
       <c r="D28" s="20">
         <f t="shared" si="0"/>
-        <v>0.03022554300188</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>-0.03022554300188</v>
+      </c>
+      <c r="E28" s="20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29" s="20">
         <v>0.335</v>
@@ -2434,12 +2506,15 @@
       </c>
       <c r="D29" s="20">
         <f t="shared" si="0"/>
-        <v>0.0304164930391857</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>-0.0304164930391857</v>
+      </c>
+      <c r="E29" s="20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30" s="20">
         <v>0.335</v>
@@ -2451,10 +2526,13 @@
         <f t="shared" si="0"/>
         <v>0.0300369755168612</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" s="20">
         <v>0.335</v>
@@ -2466,10 +2544,13 @@
         <f t="shared" si="0"/>
         <v>0.0300369755168612</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B32" s="20">
         <v>0.335</v>
@@ -2481,10 +2562,13 @@
         <f t="shared" si="0"/>
         <v>0.0296609164036732</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33" s="20">
         <v>0.335</v>
@@ -2496,10 +2580,13 @@
         <f t="shared" si="0"/>
         <v>0.030609871071223</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34" s="20">
         <v>0.335</v>
@@ -2511,10 +2598,13 @@
         <f t="shared" si="0"/>
         <v>0.0292999079982889</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" s="20">
         <v>0.335</v>
@@ -2523,13 +2613,16 @@
         <v>10.0623867981485</v>
       </c>
       <c r="D35" s="20">
-        <f t="shared" ref="D35:D53" si="1">C35/1000/B35</f>
+        <f t="shared" ref="D35:D53" si="1">C35/1000/B35*E35</f>
         <v>0.0300369755168612</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36" s="20">
         <v>0.335</v>
@@ -2541,10 +2634,13 @@
         <f t="shared" si="1"/>
         <v>0.029479307000451</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37" s="20">
         <v>0.335</v>
@@ -2556,10 +2652,13 @@
         <f t="shared" si="1"/>
         <v>0.0304164930391857</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B38" s="20">
         <v>0.335</v>
@@ -2571,10 +2670,13 @@
         <f t="shared" si="1"/>
         <v>0.0298447773131941</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B39" s="20">
         <v>0.335</v>
@@ -2586,10 +2688,13 @@
         <f t="shared" si="1"/>
         <v>0.029479307000451</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B40" s="20">
         <v>0.335</v>
@@ -2601,10 +2706,13 @@
         <f t="shared" si="1"/>
         <v>0.029479307000451</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B41" s="20">
         <v>0.335</v>
@@ -2616,10 +2724,13 @@
         <f t="shared" si="1"/>
         <v>0.0298447773131941</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B42" s="20">
         <v>0.335</v>
@@ -2629,12 +2740,15 @@
       </c>
       <c r="D42" s="20">
         <f t="shared" si="1"/>
-        <v>0.03022554300188</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>-0.03022554300188</v>
+      </c>
+      <c r="E42" s="20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43" s="20">
         <v>0.335</v>
@@ -2644,12 +2758,15 @@
       </c>
       <c r="D43" s="20">
         <f t="shared" si="1"/>
-        <v>0.0296609164036732</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>-0.0296609164036732</v>
+      </c>
+      <c r="E43" s="20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B44" s="20">
         <v>0.335</v>
@@ -2659,12 +2776,15 @@
       </c>
       <c r="D44" s="20">
         <f t="shared" si="1"/>
-        <v>0.029479307000451</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>-0.029479307000451</v>
+      </c>
+      <c r="E44" s="20">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B45" s="20">
         <v>0.4484</v>
@@ -2676,10 +2796,13 @@
         <f t="shared" si="1"/>
         <v>0.0224406485239708</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B46" s="20">
         <v>0.4484</v>
@@ -2691,10 +2814,13 @@
         <f t="shared" si="1"/>
         <v>0.0228686592525863</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B47" s="20">
         <v>0.4484</v>
@@ -2706,10 +2832,13 @@
         <f t="shared" si="1"/>
         <v>0.022024013927634</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B48" s="20">
         <v>0.4484</v>
@@ -2721,10 +2850,13 @@
         <f t="shared" si="1"/>
         <v>0.0228686592525863</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B49" s="20">
         <v>0.4484</v>
@@ -2736,10 +2868,13 @@
         <f t="shared" si="1"/>
         <v>0.022024013927634</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B50" s="20">
         <v>0.4484</v>
@@ -2751,10 +2886,13 @@
         <f t="shared" si="1"/>
         <v>0.0224768358225379</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B51" s="20">
         <v>0.4484</v>
@@ -2766,10 +2904,13 @@
         <f t="shared" si="1"/>
         <v>0.0220588689447302</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B52" s="20">
         <v>0.4484</v>
@@ -2781,10 +2922,13 @@
         <f t="shared" si="1"/>
         <v>0.0220588689447302</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B53" s="20">
         <v>0.4484</v>
@@ -2795,6 +2939,9 @@
       <c r="D53" s="20">
         <f t="shared" si="1"/>
         <v>0.0233572648754946</v>
+      </c>
+      <c r="E53" s="20">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2807,22 +2954,23 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="9" style="20"/>
     <col min="2" max="2" width="12.1333333333333" style="20" customWidth="1"/>
     <col min="3" max="3" width="9" style="20"/>
     <col min="4" max="4" width="15.6333333333333" style="20" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="20"/>
+    <col min="5" max="5" width="13.375" style="25" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" s="20" customFormat="1" spans="1:4">
+    <row r="1" s="20" customFormat="1" spans="1:5">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -2835,10 +2983,13 @@
       <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" s="20" customFormat="1" spans="1:4">
+      <c r="E1" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" s="20" customFormat="1" spans="1:5">
       <c r="A2" s="20" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2" s="20">
         <v>0.1</v>
@@ -2847,13 +2998,16 @@
         <v>2.02839756592292</v>
       </c>
       <c r="D2" s="20">
-        <f>C2/1000/B2</f>
-        <v>0.0202839756592292</v>
-      </c>
-    </row>
-    <row r="3" s="20" customFormat="1" spans="1:4">
+        <f>C2/1000/B2*E2</f>
+        <v>-0.0202839756592292</v>
+      </c>
+      <c r="E2" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" s="20" customFormat="1" spans="1:5">
       <c r="A3" s="20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B3" s="20">
         <v>0.1</v>
@@ -2862,13 +3016,16 @@
         <v>2.02839756592292</v>
       </c>
       <c r="D3" s="20">
-        <f t="shared" ref="D3:D15" si="0">C3/1000/B3</f>
-        <v>0.0202839756592292</v>
-      </c>
-    </row>
-    <row r="4" s="20" customFormat="1" spans="1:4">
+        <f t="shared" ref="D3:D49" si="0">C3/1000/B3*E3</f>
+        <v>-0.0202839756592292</v>
+      </c>
+      <c r="E3" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" s="20" customFormat="1" spans="1:5">
       <c r="A4" s="20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B4" s="20">
         <v>0.1</v>
@@ -2878,12 +3035,15 @@
       </c>
       <c r="D4" s="20">
         <f t="shared" si="0"/>
-        <v>0.0202839756592292</v>
-      </c>
-    </row>
-    <row r="5" s="20" customFormat="1" spans="1:4">
+        <v>-0.0202839756592292</v>
+      </c>
+      <c r="E4" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" s="20" customFormat="1" spans="1:5">
       <c r="A5" s="20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B5" s="20">
         <v>0.1</v>
@@ -2893,12 +3053,15 @@
       </c>
       <c r="D5" s="20">
         <f t="shared" si="0"/>
-        <v>0.0202839756592292</v>
-      </c>
-    </row>
-    <row r="6" s="20" customFormat="1" spans="1:4">
+        <v>-0.0202839756592292</v>
+      </c>
+      <c r="E5" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" s="20" customFormat="1" spans="1:5">
       <c r="A6" s="20" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B6" s="20">
         <v>0.1</v>
@@ -2908,12 +3071,15 @@
       </c>
       <c r="D6" s="20">
         <f t="shared" si="0"/>
-        <v>0.0202839756592292</v>
-      </c>
-    </row>
-    <row r="7" s="20" customFormat="1" spans="1:4">
+        <v>-0.0202839756592292</v>
+      </c>
+      <c r="E6" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" s="20" customFormat="1" spans="1:5">
       <c r="A7" s="20" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B7" s="20">
         <v>0.1</v>
@@ -2923,12 +3089,15 @@
       </c>
       <c r="D7" s="20">
         <f t="shared" si="0"/>
-        <v>0.0204081632653061</v>
-      </c>
-    </row>
-    <row r="8" s="20" customFormat="1" spans="1:4">
+        <v>-0.0204081632653061</v>
+      </c>
+      <c r="E7" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" s="20" customFormat="1" spans="1:5">
       <c r="A8" s="20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B8" s="20">
         <v>0.1</v>
@@ -2938,12 +3107,15 @@
       </c>
       <c r="D8" s="20">
         <f t="shared" si="0"/>
-        <v>0.0202839756592292</v>
-      </c>
-    </row>
-    <row r="9" s="20" customFormat="1" spans="1:4">
+        <v>-0.0202839756592292</v>
+      </c>
+      <c r="E8" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" s="20" customFormat="1" spans="1:5">
       <c r="A9" s="20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B9" s="20">
         <v>0.1</v>
@@ -2953,12 +3125,15 @@
       </c>
       <c r="D9" s="20">
         <f t="shared" si="0"/>
-        <v>0.0204123290467442</v>
-      </c>
-    </row>
-    <row r="10" s="20" customFormat="1" spans="1:4">
+        <v>-0.0204123290467442</v>
+      </c>
+      <c r="E9" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" s="20" customFormat="1" spans="1:5">
       <c r="A10" s="20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B10" s="20">
         <v>0.1</v>
@@ -2968,12 +3143,15 @@
       </c>
       <c r="D10" s="20">
         <f t="shared" si="0"/>
-        <v>0.0204123290467442</v>
-      </c>
-    </row>
-    <row r="11" s="20" customFormat="1" spans="1:4">
+        <v>-0.0204123290467442</v>
+      </c>
+      <c r="E10" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" s="20" customFormat="1" spans="1:5">
       <c r="A11" s="20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B11" s="20">
         <v>0.1</v>
@@ -2983,12 +3161,15 @@
       </c>
       <c r="D11" s="20">
         <f t="shared" si="0"/>
-        <v>0.0202839756592292</v>
-      </c>
-    </row>
-    <row r="12" s="20" customFormat="1" spans="1:4">
+        <v>-0.0202839756592292</v>
+      </c>
+      <c r="E11" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" s="20" customFormat="1" spans="1:5">
       <c r="A12" s="20" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B12" s="20">
         <v>0.1</v>
@@ -2998,12 +3179,15 @@
       </c>
       <c r="D12" s="20">
         <f t="shared" si="0"/>
-        <v>0.0202839756592292</v>
-      </c>
-    </row>
-    <row r="13" s="20" customFormat="1" spans="1:4">
+        <v>-0.0202839756592292</v>
+      </c>
+      <c r="E12" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" s="20" customFormat="1" spans="1:5">
       <c r="A13" s="20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B13" s="20">
         <v>0.1</v>
@@ -3013,12 +3197,15 @@
       </c>
       <c r="D13" s="20">
         <f t="shared" si="0"/>
-        <v>0.0204123290467442</v>
-      </c>
-    </row>
-    <row r="14" s="20" customFormat="1" spans="1:4">
+        <v>-0.0204123290467442</v>
+      </c>
+      <c r="E13" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" s="20" customFormat="1" spans="1:5">
       <c r="A14" s="20" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B14" s="20">
         <v>0.2271</v>
@@ -3028,12 +3215,15 @@
       </c>
       <c r="D14" s="20">
         <f t="shared" si="0"/>
-        <v>0.0220167327168648</v>
-      </c>
-    </row>
-    <row r="15" s="20" customFormat="1" spans="1:4">
+        <v>-0.0220167327168648</v>
+      </c>
+      <c r="E14" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" s="20" customFormat="1" spans="1:5">
       <c r="A15" s="20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B15" s="20">
         <v>0.2271</v>
@@ -3043,12 +3233,15 @@
       </c>
       <c r="D15" s="20">
         <f t="shared" si="0"/>
-        <v>0.0220123302508147</v>
-      </c>
-    </row>
-    <row r="16" s="20" customFormat="1" spans="1:4">
+        <v>-0.0220123302508147</v>
+      </c>
+      <c r="E15" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" s="20" customFormat="1" spans="1:5">
       <c r="A16" s="20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B16" s="20">
         <v>0.2271</v>
@@ -3057,13 +3250,16 @@
         <v>4.99900019996001</v>
       </c>
       <c r="D16" s="20">
-        <f t="shared" ref="D16:D49" si="1">C16/1000/B16</f>
-        <v>0.0220123302508147</v>
-      </c>
-    </row>
-    <row r="17" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.0220123302508147</v>
+      </c>
+      <c r="E16" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" s="20" customFormat="1" spans="1:5">
       <c r="A17" s="20" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B17" s="20">
         <v>0.2271</v>
@@ -3072,13 +3268,16 @@
         <v>4.99900019996001</v>
       </c>
       <c r="D17" s="20">
-        <f t="shared" si="1"/>
-        <v>0.0220123302508147</v>
-      </c>
-    </row>
-    <row r="18" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.0220123302508147</v>
+      </c>
+      <c r="E17" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" s="20" customFormat="1" spans="1:5">
       <c r="A18" s="20" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B18" s="20">
         <v>0.2271</v>
@@ -3087,13 +3286,16 @@
         <v>4.99900019996001</v>
       </c>
       <c r="D18" s="20">
-        <f t="shared" si="1"/>
-        <v>0.0220123302508147</v>
-      </c>
-    </row>
-    <row r="19" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.0220123302508147</v>
+      </c>
+      <c r="E18" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" s="20" customFormat="1" spans="1:5">
       <c r="A19" s="20" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B19" s="20">
         <v>0.2271</v>
@@ -3102,13 +3304,16 @@
         <v>5.09476258406358</v>
       </c>
       <c r="D19" s="20">
-        <f t="shared" si="1"/>
-        <v>0.0224340052138423</v>
-      </c>
-    </row>
-    <row r="20" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.0224340052138423</v>
+      </c>
+      <c r="E19" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" s="20" customFormat="1" spans="1:5">
       <c r="A20" s="20" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B20" s="20">
         <v>0.2271</v>
@@ -3117,13 +3322,16 @@
         <v>4.96820349761526</v>
       </c>
       <c r="D20" s="20">
-        <f t="shared" si="1"/>
-        <v>0.0218767216979976</v>
-      </c>
-    </row>
-    <row r="21" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.0218767216979976</v>
+      </c>
+      <c r="E20" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" s="20" customFormat="1" spans="1:5">
       <c r="A21" s="20" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B21" s="20">
         <v>0.2271</v>
@@ -3132,13 +3340,16 @@
         <v>5.09476258406358</v>
       </c>
       <c r="D21" s="20">
-        <f t="shared" si="1"/>
-        <v>0.0224340052138423</v>
-      </c>
-    </row>
-    <row r="22" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.0224340052138423</v>
+      </c>
+      <c r="E21" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" s="20" customFormat="1" spans="1:5">
       <c r="A22" s="20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B22" s="20">
         <v>0.2271</v>
@@ -3147,413 +3358,497 @@
         <v>4.93778392257555</v>
       </c>
       <c r="D22" s="20">
-        <f t="shared" si="1"/>
-        <v>0.0217427737673956</v>
-      </c>
-    </row>
-    <row r="23" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.0217427737673956</v>
+      </c>
+      <c r="E22" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" s="20" customFormat="1" spans="1:5">
       <c r="A23" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="28">
+        <v>79</v>
+      </c>
+      <c r="B23" s="26">
         <v>0.726</v>
       </c>
       <c r="C23" s="20">
         <v>10.0623867981485</v>
       </c>
       <c r="D23" s="20">
-        <f t="shared" si="1"/>
-        <v>0.0138600369120503</v>
-      </c>
-    </row>
-    <row r="24" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.0138600369120503</v>
+      </c>
+      <c r="E23" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" s="20" customFormat="1" spans="1:5">
       <c r="A24" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="28">
+        <v>80</v>
+      </c>
+      <c r="B24" s="26">
         <v>0.726</v>
       </c>
       <c r="C24" s="20">
         <v>10.0623867981485</v>
       </c>
       <c r="D24" s="20">
-        <f t="shared" si="1"/>
-        <v>0.0138600369120503</v>
-      </c>
-    </row>
-    <row r="25" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.0138600369120503</v>
+      </c>
+      <c r="E24" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" s="20" customFormat="1" spans="1:5">
       <c r="A25" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="28">
+        <v>81</v>
+      </c>
+      <c r="B25" s="26">
         <v>0.726</v>
       </c>
       <c r="C25" s="20">
         <v>10.0623867981485</v>
       </c>
       <c r="D25" s="20">
-        <f t="shared" si="1"/>
-        <v>0.0138600369120503</v>
-      </c>
-    </row>
-    <row r="26" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.0138600369120503</v>
+      </c>
+      <c r="E25" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" s="20" customFormat="1" spans="1:5">
       <c r="A26" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" s="28">
+        <v>82</v>
+      </c>
+      <c r="B26" s="26">
         <v>0.726</v>
       </c>
       <c r="C26" s="20">
         <v>4.96820349761526</v>
       </c>
       <c r="D26" s="20">
-        <f t="shared" si="1"/>
-        <v>0.00684325550635711</v>
-      </c>
-    </row>
-    <row r="27" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.00684325550635711</v>
+      </c>
+      <c r="E26" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" s="20" customFormat="1" spans="1:5">
       <c r="A27" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="28">
+        <v>83</v>
+      </c>
+      <c r="B27" s="26">
         <v>0.726</v>
       </c>
       <c r="C27" s="20">
         <v>4.96820349761526</v>
       </c>
       <c r="D27" s="20">
-        <f t="shared" si="1"/>
-        <v>0.00684325550635711</v>
-      </c>
-    </row>
-    <row r="28" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.00684325550635711</v>
+      </c>
+      <c r="E27" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" s="20" customFormat="1" spans="1:5">
       <c r="A28" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="28">
+        <v>84</v>
+      </c>
+      <c r="B28" s="26">
         <v>0.726</v>
       </c>
       <c r="C28" s="20">
         <v>4.96820349761526</v>
       </c>
       <c r="D28" s="20">
-        <f t="shared" si="1"/>
-        <v>0.00684325550635711</v>
-      </c>
-    </row>
-    <row r="29" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.00684325550635711</v>
+      </c>
+      <c r="E28" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" s="20" customFormat="1" spans="1:5">
       <c r="A29" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B29" s="28">
+        <v>85</v>
+      </c>
+      <c r="B29" s="26">
         <v>0.726</v>
       </c>
       <c r="C29" s="20">
         <v>5.06277845281491</v>
       </c>
       <c r="D29" s="20">
-        <f t="shared" si="1"/>
-        <v>0.00697352403968996</v>
-      </c>
-    </row>
-    <row r="30" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.00697352403968996</v>
+      </c>
+      <c r="E29" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" s="20" customFormat="1" spans="1:5">
       <c r="A30" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" s="28">
+        <v>86</v>
+      </c>
+      <c r="B30" s="26">
         <v>0.726</v>
       </c>
       <c r="C30" s="20">
         <v>4.93778392257555</v>
       </c>
       <c r="D30" s="20">
-        <f t="shared" si="1"/>
-        <v>0.00680135526525558</v>
-      </c>
-    </row>
-    <row r="31" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.00680135526525558</v>
+      </c>
+      <c r="E30" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" s="20" customFormat="1" spans="1:5">
       <c r="A31" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="B31" s="28">
+        <v>87</v>
+      </c>
+      <c r="B31" s="26">
         <v>0.726</v>
       </c>
       <c r="C31" s="20">
         <v>5.09476258406358</v>
       </c>
       <c r="D31" s="20">
-        <f t="shared" si="1"/>
-        <v>0.00701757931689198</v>
-      </c>
-    </row>
-    <row r="32" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.00701757931689198</v>
+      </c>
+      <c r="E31" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" s="20" customFormat="1" spans="1:5">
       <c r="A32" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B32" s="28">
+        <v>88</v>
+      </c>
+      <c r="B32" s="26">
         <v>0.726</v>
       </c>
       <c r="C32" s="20">
         <v>5.06277845281491</v>
       </c>
       <c r="D32" s="20">
-        <f t="shared" si="1"/>
-        <v>0.00697352403968996</v>
-      </c>
-    </row>
-    <row r="33" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.00697352403968996</v>
+      </c>
+      <c r="E32" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" s="20" customFormat="1" spans="1:5">
       <c r="A33" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B33" s="28">
+        <v>89</v>
+      </c>
+      <c r="B33" s="26">
         <v>0.726</v>
       </c>
       <c r="C33" s="20">
         <v>5.15995872033024</v>
       </c>
       <c r="D33" s="20">
-        <f t="shared" si="1"/>
-        <v>0.00710738115747967</v>
-      </c>
-    </row>
-    <row r="34" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.00710738115747967</v>
+      </c>
+      <c r="E33" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" s="20" customFormat="1" spans="1:5">
       <c r="A34" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B34" s="28">
+        <v>90</v>
+      </c>
+      <c r="B34" s="26">
         <v>0.726</v>
       </c>
       <c r="C34" s="20">
         <v>5.0709939148073</v>
       </c>
       <c r="D34" s="20">
-        <f>-C34/1000/B34</f>
-        <v>-0.00698484010304036</v>
-      </c>
-    </row>
-    <row r="35" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>0.00698484010304036</v>
+      </c>
+      <c r="E34" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" s="20" customFormat="1" spans="1:5">
       <c r="A35" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B35" s="28">
+        <v>91</v>
+      </c>
+      <c r="B35" s="26">
         <v>0.726</v>
       </c>
       <c r="C35" s="20">
         <v>5.0709939148073</v>
       </c>
       <c r="D35" s="20">
-        <f>-C35/1000/B35</f>
-        <v>-0.00698484010304036</v>
-      </c>
-    </row>
-    <row r="36" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>0.00698484010304036</v>
+      </c>
+      <c r="E35" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" s="20" customFormat="1" spans="1:5">
       <c r="A36" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="B36" s="28">
+        <v>92</v>
+      </c>
+      <c r="B36" s="26">
         <v>0.726</v>
       </c>
       <c r="C36" s="20">
         <v>5.03930659141302</v>
       </c>
       <c r="D36" s="20">
-        <f>-C36/1000/B36</f>
-        <v>-0.00694119365208405</v>
-      </c>
-    </row>
-    <row r="37" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>0.00694119365208405</v>
+      </c>
+      <c r="E36" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" s="20" customFormat="1" spans="1:5">
       <c r="A37" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B37" s="28">
+        <v>93</v>
+      </c>
+      <c r="B37" s="26">
         <v>0.726</v>
       </c>
       <c r="C37" s="20">
         <v>5.03930659141302</v>
       </c>
       <c r="D37" s="20">
-        <f>-C37/1000/B37</f>
-        <v>-0.00694119365208405</v>
-      </c>
-    </row>
-    <row r="38" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>0.00694119365208405</v>
+      </c>
+      <c r="E37" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" s="20" customFormat="1" spans="1:5">
       <c r="A38" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B38" s="28">
+        <v>94</v>
+      </c>
+      <c r="B38" s="26">
         <v>0.726</v>
       </c>
-      <c r="C38" s="29">
+      <c r="C38" s="27">
         <v>9.71345313258863</v>
       </c>
       <c r="D38" s="20">
-        <f t="shared" si="1"/>
-        <v>0.013379412028359</v>
-      </c>
-    </row>
-    <row r="39" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.013379412028359</v>
+      </c>
+      <c r="E38" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" s="20" customFormat="1" spans="1:5">
       <c r="A39" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B39" s="28">
+        <v>95</v>
+      </c>
+      <c r="B39" s="26">
         <v>0.726</v>
       </c>
-      <c r="C39" s="29">
+      <c r="C39" s="27">
         <v>10.1729399796541</v>
       </c>
       <c r="D39" s="20">
-        <f t="shared" si="1"/>
-        <v>0.0140123140215621</v>
-      </c>
-    </row>
-    <row r="40" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.0140123140215621</v>
+      </c>
+      <c r="E39" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" s="20" customFormat="1" spans="1:5">
       <c r="A40" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B40" s="28">
+        <v>96</v>
+      </c>
+      <c r="B40" s="26">
         <v>0.726</v>
       </c>
-      <c r="C40" s="29">
+      <c r="C40" s="27">
         <v>10.1729399796541</v>
       </c>
       <c r="D40" s="20">
-        <f t="shared" si="1"/>
-        <v>0.0140123140215621</v>
-      </c>
-    </row>
-    <row r="41" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>-0.0140123140215621</v>
+      </c>
+      <c r="E40" s="25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" s="20" customFormat="1" spans="1:5">
       <c r="A41" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="B41" s="28">
+        <v>97</v>
+      </c>
+      <c r="B41" s="26">
         <v>0.2271</v>
       </c>
       <c r="C41" s="20">
         <v>5.0709939148073</v>
       </c>
       <c r="D41" s="20">
-        <f t="shared" ref="D41:D49" si="2">-C41/1000/B41</f>
-        <v>-0.0223293435262321</v>
-      </c>
-    </row>
-    <row r="42" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>0.0223293435262321</v>
+      </c>
+      <c r="E41" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" s="20" customFormat="1" spans="1:5">
       <c r="A42" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B42" s="28">
+        <v>98</v>
+      </c>
+      <c r="B42" s="26">
         <v>0.2271</v>
       </c>
       <c r="C42" s="20">
         <v>5.0709939148073</v>
       </c>
       <c r="D42" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.0223293435262321</v>
-      </c>
-    </row>
-    <row r="43" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>0.0223293435262321</v>
+      </c>
+      <c r="E42" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" s="20" customFormat="1" spans="1:5">
       <c r="A43" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="B43" s="28">
+        <v>99</v>
+      </c>
+      <c r="B43" s="26">
         <v>0.2271</v>
       </c>
       <c r="C43" s="20">
         <v>5.0709939148073</v>
       </c>
       <c r="D43" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.0223293435262321</v>
-      </c>
-    </row>
-    <row r="44" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>0.0223293435262321</v>
+      </c>
+      <c r="E43" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" s="20" customFormat="1" spans="1:5">
       <c r="A44" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="B44" s="28">
+        <v>100</v>
+      </c>
+      <c r="B44" s="26">
         <v>0.2271</v>
       </c>
       <c r="C44" s="20">
         <v>5.0709939148073</v>
       </c>
       <c r="D44" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.0223293435262321</v>
-      </c>
-    </row>
-    <row r="45" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>0.0223293435262321</v>
+      </c>
+      <c r="E44" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" s="20" customFormat="1" spans="1:5">
       <c r="A45" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="28">
+        <v>101</v>
+      </c>
+      <c r="B45" s="26">
         <v>0.2271</v>
       </c>
       <c r="C45" s="20">
         <v>5.0709939148073</v>
       </c>
       <c r="D45" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.0223293435262321</v>
-      </c>
-    </row>
-    <row r="46" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>0.0223293435262321</v>
+      </c>
+      <c r="E45" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" s="20" customFormat="1" spans="1:5">
       <c r="A46" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" s="28">
+        <v>102</v>
+      </c>
+      <c r="B46" s="26">
         <v>0.2271</v>
       </c>
       <c r="C46" s="20">
         <v>5.0709939148073</v>
       </c>
       <c r="D46" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.0223293435262321</v>
-      </c>
-    </row>
-    <row r="47" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>0.0223293435262321</v>
+      </c>
+      <c r="E46" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" s="20" customFormat="1" spans="1:5">
       <c r="A47" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B47" s="28">
+        <v>103</v>
+      </c>
+      <c r="B47" s="26">
         <v>0.2271</v>
       </c>
       <c r="C47" s="20">
         <v>5.0709939148073</v>
       </c>
       <c r="D47" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.0223293435262321</v>
-      </c>
-    </row>
-    <row r="48" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>0.0223293435262321</v>
+      </c>
+      <c r="E47" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" s="20" customFormat="1" spans="1:5">
       <c r="A48" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="B48" s="28">
+        <v>104</v>
+      </c>
+      <c r="B48" s="26">
         <v>0.2271</v>
       </c>
       <c r="C48" s="20">
         <v>5.03930659141302</v>
       </c>
       <c r="D48" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.0221898132602951</v>
-      </c>
-    </row>
-    <row r="49" s="20" customFormat="1" spans="1:4">
+        <f t="shared" si="0"/>
+        <v>0.0221898132602951</v>
+      </c>
+      <c r="E48" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" s="20" customFormat="1" spans="1:5">
       <c r="A49" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="B49" s="28">
+        <v>105</v>
+      </c>
+      <c r="B49" s="26">
         <v>0.2271</v>
       </c>
       <c r="C49" s="20">
         <v>5.0709939148073</v>
       </c>
       <c r="D49" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.0223293435262321</v>
+        <f t="shared" si="0"/>
+        <v>0.0223293435262321</v>
+      </c>
+      <c r="E49" s="25">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3566,39 +3861,38 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="$A15:$XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="13.3833333333333" style="20" customWidth="1"/>
     <col min="2" max="2" width="11.3833333333333" style="20" customWidth="1"/>
     <col min="3" max="3" width="11.1333333333333" style="20" customWidth="1"/>
-    <col min="4" max="4" width="9.44166666666667" style="20"/>
-    <col min="5" max="5" width="8.63333333333333" style="20" customWidth="1"/>
-    <col min="6" max="6" width="9" style="20"/>
-    <col min="7" max="7" width="12.3833333333333" style="20" customWidth="1"/>
-    <col min="8" max="8" width="14.1083333333333" style="20"/>
-    <col min="9" max="16384" width="9" style="20"/>
+    <col min="4" max="4" width="27.5" style="20" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" ht="14.25" spans="1:7">
+        <v>107</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="20" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B2" s="20">
         <v>500.951808436029</v>
@@ -3607,22 +3901,12 @@
         <v>-0.0834919680726715</v>
       </c>
       <c r="D2" s="21">
-        <v>500.951808436029</v>
-      </c>
-      <c r="E2" s="22">
-        <f>D2/1000/6</f>
-        <v>0.0834919680726715</v>
-      </c>
-      <c r="F2" s="20">
-        <v>-0.085</v>
-      </c>
-      <c r="G2" s="23">
-        <v>1.05141289587297</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" spans="1:7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="20" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B3" s="20">
         <v>508.854060655404</v>
@@ -3631,22 +3915,12 @@
         <v>0.084809010109234</v>
       </c>
       <c r="D3" s="21">
-        <v>508.854060655404</v>
-      </c>
-      <c r="E3" s="22">
-        <f t="shared" ref="E3:E20" si="0">D3/1000/6</f>
-        <v>0.084809010109234</v>
-      </c>
-      <c r="F3" s="20">
-        <v>0.085</v>
-      </c>
-      <c r="G3" s="23">
-        <v>1.04497421034587</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="20" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B4" s="20">
         <v>508.854060655404</v>
@@ -3655,22 +3929,12 @@
         <v>0.084809010109234</v>
       </c>
       <c r="D4" s="21">
-        <v>508.854060655404</v>
-      </c>
-      <c r="E4" s="22">
-        <f t="shared" si="0"/>
-        <v>0.084809010109234</v>
-      </c>
-      <c r="F4" s="20">
-        <v>0.085</v>
-      </c>
-      <c r="G4" s="23">
-        <v>1.02510720127584</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="20" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B5" s="20">
         <v>507.150826655847</v>
@@ -3679,22 +3943,12 @@
         <v>0.0845251377759745</v>
       </c>
       <c r="D5" s="21">
-        <v>507.150826655847</v>
-      </c>
-      <c r="E5" s="22">
-        <f t="shared" si="0"/>
-        <v>0.0845251377759745</v>
-      </c>
-      <c r="F5" s="20">
-        <v>0.085</v>
-      </c>
-      <c r="G5" s="23">
-        <v>0.985542533840889</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="20" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B6" s="20">
         <v>494.559841740851</v>
@@ -3703,22 +3957,12 @@
         <v>-0.0824266402901418</v>
       </c>
       <c r="D6" s="21">
-        <v>494.559841740851</v>
-      </c>
-      <c r="E6" s="22">
-        <f t="shared" si="0"/>
-        <v>0.0824266402901418</v>
-      </c>
-      <c r="F6" s="20">
-        <v>-0.085</v>
-      </c>
-      <c r="G6" s="23">
-        <v>1.00790267040447</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25" spans="1:7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="20" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B7" s="20">
         <v>503.981453482512</v>
@@ -3727,22 +3971,12 @@
         <v>-0.083996908913752</v>
       </c>
       <c r="D7" s="21">
-        <v>503.981453482512</v>
-      </c>
-      <c r="E7" s="22">
-        <f t="shared" si="0"/>
-        <v>0.083996908913752</v>
-      </c>
-      <c r="F7" s="20">
-        <v>-0.085</v>
-      </c>
-      <c r="G7" s="23">
-        <v>0.96769087183098</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25" spans="1:7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="20" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B8" s="20">
         <v>477.099236641221</v>
@@ -3751,22 +3985,12 @@
         <v>-0.0795165394402035</v>
       </c>
       <c r="D8" s="21">
-        <v>477.099236641221</v>
-      </c>
-      <c r="E8" s="22">
-        <f t="shared" si="0"/>
-        <v>0.0795165394402035</v>
-      </c>
-      <c r="F8" s="20">
-        <v>-0.085</v>
-      </c>
-      <c r="G8" s="23">
-        <v>1.03246933791451</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25" spans="1:7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="20" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B9" s="20">
         <v>503.981453482512</v>
@@ -3775,22 +3999,12 @@
         <v>0.083996908913752</v>
       </c>
       <c r="D9" s="21">
-        <v>503.981453482512</v>
-      </c>
-      <c r="E9" s="22">
-        <f t="shared" si="0"/>
-        <v>0.083996908913752</v>
-      </c>
-      <c r="F9" s="20">
-        <v>0.085</v>
-      </c>
-      <c r="G9" s="23">
-        <v>1.03552235408932</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="20" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B10" s="20">
         <v>503.981453482512</v>
@@ -3799,22 +4013,12 @@
         <v>-0.083996908913752</v>
       </c>
       <c r="D10" s="21">
-        <v>503.981453482512</v>
-      </c>
-      <c r="E10" s="22">
-        <f t="shared" si="0"/>
-        <v>0.083996908913752</v>
-      </c>
-      <c r="F10" s="20">
-        <v>-0.085</v>
-      </c>
-      <c r="G10" s="24">
-        <v>1.30718497829121</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25" spans="1:7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="20" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B11" s="20">
         <v>491.642084562439</v>
@@ -3823,22 +4027,12 @@
         <v>-0.0819403474270732</v>
       </c>
       <c r="D11" s="21">
-        <v>491.642084562439</v>
-      </c>
-      <c r="E11" s="22">
-        <f t="shared" si="0"/>
-        <v>0.0819403474270732</v>
-      </c>
-      <c r="F11" s="20">
-        <v>-0.085</v>
-      </c>
-      <c r="G11" s="24">
-        <v>1.58590805403929</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25" spans="1:7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="20" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B12" s="20">
         <v>494.559841740851</v>
@@ -3847,22 +4041,12 @@
         <v>-0.0824266402901418</v>
       </c>
       <c r="D12" s="21">
-        <v>494.559841740851</v>
-      </c>
-      <c r="E12" s="22">
-        <f t="shared" si="0"/>
-        <v>0.0824266402901418</v>
-      </c>
-      <c r="F12" s="20">
-        <v>-0.085</v>
-      </c>
-      <c r="G12" s="24">
-        <v>1.16091508958913</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25" spans="1:7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="20" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B13" s="20">
         <v>503.981453482512</v>
@@ -3871,22 +4055,12 @@
         <v>-0.083996908913752</v>
       </c>
       <c r="D13" s="21">
-        <v>503.981453482512</v>
-      </c>
-      <c r="E13" s="22">
-        <f t="shared" si="0"/>
-        <v>0.083996908913752</v>
-      </c>
-      <c r="F13" s="20">
-        <v>-0.085</v>
-      </c>
-      <c r="G13" s="23">
-        <v>0.999311540469612</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25" spans="1:7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="20" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B14" s="20">
         <v>513.663447709061</v>
@@ -3895,22 +4069,12 @@
         <v>0.0856105746181768</v>
       </c>
       <c r="D14" s="21">
-        <v>513.663447709061</v>
-      </c>
-      <c r="E14" s="22">
-        <f t="shared" si="0"/>
-        <v>0.0856105746181768</v>
-      </c>
-      <c r="F14" s="20">
-        <v>0.085</v>
-      </c>
-      <c r="G14" s="23">
-        <v>0.954487879262718</v>
-      </c>
-    </row>
-    <row r="15" ht="14.25" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="20" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B15" s="20">
         <v>503.981453482512</v>
@@ -3919,22 +4083,12 @@
         <v>-0.083996908913752</v>
       </c>
       <c r="D15" s="21">
-        <v>503.981453482512</v>
-      </c>
-      <c r="E15" s="22">
-        <f t="shared" si="0"/>
-        <v>0.083996908913752</v>
-      </c>
-      <c r="F15" s="20">
-        <v>-0.085</v>
-      </c>
-      <c r="G15" s="23">
-        <v>0.982295081018815</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25" spans="1:7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="20" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B16" s="20">
         <v>513.663447709061</v>
@@ -3943,22 +4097,12 @@
         <v>0.0856105746181768</v>
       </c>
       <c r="D16" s="21">
-        <v>513.663447709061</v>
-      </c>
-      <c r="E16" s="22">
-        <f t="shared" si="0"/>
-        <v>0.0856105746181768</v>
-      </c>
-      <c r="F16" s="20">
-        <v>0.085</v>
-      </c>
-      <c r="G16" s="23">
-        <v>0.97702070710649</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="20" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B17" s="20">
         <v>513.663447709061</v>
@@ -3967,22 +4111,12 @@
         <v>0.0856105746181768</v>
       </c>
       <c r="D17" s="21">
-        <v>513.663447709061</v>
-      </c>
-      <c r="E17" s="22">
-        <f t="shared" si="0"/>
-        <v>0.0856105746181768</v>
-      </c>
-      <c r="F17" s="20">
-        <v>0.085</v>
-      </c>
-      <c r="G17" s="23">
-        <v>0.9479618744931</v>
-      </c>
-    </row>
-    <row r="18" ht="14.25" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="20" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B18" s="20">
         <v>503.981453482512</v>
@@ -3991,22 +4125,12 @@
         <v>-0.083996908913752</v>
       </c>
       <c r="D18" s="21">
-        <v>503.981453482512</v>
-      </c>
-      <c r="E18" s="22">
-        <f t="shared" si="0"/>
-        <v>0.083996908913752</v>
-      </c>
-      <c r="F18" s="20">
-        <v>-0.085</v>
-      </c>
-      <c r="G18" s="23">
-        <v>0.792927641006873</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25" spans="1:7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="20" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B19" s="20">
         <v>510.41241322989</v>
@@ -4015,22 +4139,12 @@
         <v>0.085068735538315</v>
       </c>
       <c r="D19" s="21">
-        <v>510.41241322989</v>
-      </c>
-      <c r="E19" s="22">
-        <f t="shared" si="0"/>
-        <v>0.085068735538315</v>
-      </c>
-      <c r="F19" s="20">
-        <v>0.085</v>
-      </c>
-      <c r="G19" s="23">
-        <v>0.936397974673713</v>
-      </c>
-    </row>
-    <row r="20" ht="14.25" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="20" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B20" s="20">
         <v>494.559841740851</v>
@@ -4039,22 +4153,12 @@
         <v>-0.0824266402901418</v>
       </c>
       <c r="D20" s="21">
-        <v>494.559841740851</v>
-      </c>
-      <c r="E20" s="22">
-        <f t="shared" si="0"/>
-        <v>0.0824266402901418</v>
-      </c>
-      <c r="F20" s="20">
-        <v>-0.085</v>
-      </c>
-      <c r="G20" s="23">
-        <v>0.984456916873171</v>
-      </c>
-    </row>
-    <row r="21" ht="14.25" spans="1:7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="20" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B21" s="20">
         <v>98.9119683481701</v>
@@ -4063,450 +4167,372 @@
         <f>-B21/1000</f>
         <v>-0.0989119683481701</v>
       </c>
-      <c r="F21" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G21" s="23">
-        <v>0.963505342010869</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25" spans="1:7">
+      <c r="D21" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="20" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B22" s="20">
         <v>99.5024875621891</v>
       </c>
       <c r="C22" s="20">
-        <f t="shared" ref="C22:C30" si="1">-B22/1000</f>
+        <f t="shared" ref="C22:C30" si="0">-B22/1000</f>
         <v>-0.0995024875621891</v>
       </c>
-      <c r="F22" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G22" s="23">
-        <v>0.954644492227053</v>
-      </c>
-    </row>
-    <row r="23" ht="14.25" spans="1:7">
+      <c r="D22" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="20" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B23" s="20">
         <v>98.9119683481701</v>
       </c>
       <c r="C23" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.0989119683481701</v>
+      </c>
+      <c r="D23" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" s="20">
+        <v>98.9119683481701</v>
+      </c>
+      <c r="C24" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.0989119683481701</v>
+      </c>
+      <c r="D24" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="20">
+        <v>97.0873786407767</v>
+      </c>
+      <c r="C25" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.0970873786407767</v>
+      </c>
+      <c r="D25" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="20">
+        <v>98.9119683481701</v>
+      </c>
+      <c r="C26" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.0989119683481701</v>
+      </c>
+      <c r="D26" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="20">
+        <v>95.4198473282443</v>
+      </c>
+      <c r="C27" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.0954198473282443</v>
+      </c>
+      <c r="D27" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" s="20">
+        <v>100.796290696502</v>
+      </c>
+      <c r="C28" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.100796290696502</v>
+      </c>
+      <c r="D28" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" s="20">
+        <v>99.5024875621891</v>
+      </c>
+      <c r="C29" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.0995024875621891</v>
+      </c>
+      <c r="D29" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30" s="20">
+        <v>97.0873786407767</v>
+      </c>
+      <c r="C30" s="20">
+        <f t="shared" si="0"/>
+        <v>-0.0970873786407767</v>
+      </c>
+      <c r="D30" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" s="20">
+        <v>314.267756128221</v>
+      </c>
+      <c r="C31" s="20">
+        <f t="shared" ref="C31:C48" si="1">-B31/1000</f>
+        <v>-0.314267756128221</v>
+      </c>
+      <c r="D31" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="20">
+        <v>304.692260816575</v>
+      </c>
+      <c r="C32" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.304692260816575</v>
+      </c>
+      <c r="D32" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33" s="20">
+        <v>293.427230046948</v>
+      </c>
+      <c r="C33" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.293427230046948</v>
+      </c>
+      <c r="D33" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="23">
+        <v>296.73590504451</v>
+      </c>
+      <c r="C34" s="20">
+        <f>B34/1000</f>
+        <v>0.29673590504451</v>
+      </c>
+      <c r="D34" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" s="23">
+        <v>296.73590504451</v>
+      </c>
+      <c r="C35" s="24">
+        <f t="shared" si="1"/>
+        <v>-0.29673590504451</v>
+      </c>
+      <c r="D35" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" s="20">
+        <v>293.427230046948</v>
+      </c>
+      <c r="C36" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.293427230046948</v>
+      </c>
+      <c r="D36" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" s="20">
+        <v>285.225328009127</v>
+      </c>
+      <c r="C37" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.285225328009127</v>
+      </c>
+      <c r="D37" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="20">
+        <v>314.267756128221</v>
+      </c>
+      <c r="C38" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.314267756128221</v>
+      </c>
+      <c r="D38" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" s="20">
+        <v>100.78613182826</v>
+      </c>
+      <c r="C39" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.10078613182826</v>
+      </c>
+      <c r="D39" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B40" s="20">
+        <v>99.5421063109695</v>
+      </c>
+      <c r="C40" s="20">
+        <f t="shared" si="1"/>
+        <v>-0.0995421063109695</v>
+      </c>
+      <c r="D40" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" s="20">
+        <v>98.9119683481701</v>
+      </c>
+      <c r="C41" s="20">
         <f t="shared" si="1"/>
         <v>-0.0989119683481701</v>
       </c>
-      <c r="F23" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G23" s="23">
-        <v>0.987926729944811</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25" spans="1:7">
-      <c r="A24" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="B24" s="20">
+      <c r="D41" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B42" s="20">
         <v>98.9119683481701</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C42" s="20">
         <f t="shared" si="1"/>
         <v>-0.0989119683481701</v>
       </c>
-      <c r="F24" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G24" s="23">
-        <v>1.0059675104667</v>
-      </c>
-    </row>
-    <row r="25" ht="14.25" spans="1:7">
-      <c r="A25" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="B25" s="20">
-        <v>97.0873786407767</v>
-      </c>
-      <c r="C25" s="20">
-        <f t="shared" si="1"/>
-        <v>-0.0970873786407767</v>
-      </c>
-      <c r="F25" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G25" s="23">
-        <v>0.959971805022039</v>
-      </c>
-    </row>
-    <row r="26" ht="14.25" spans="1:7">
-      <c r="A26" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B26" s="20">
+      <c r="D42" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" s="20">
         <v>98.9119683481701</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C43" s="20">
         <f t="shared" si="1"/>
         <v>-0.0989119683481701</v>
       </c>
-      <c r="F26" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G26" s="23">
-        <v>0.967885395533345</v>
-      </c>
-    </row>
-    <row r="27" ht="14.25" spans="1:7">
-      <c r="A27" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="B27" s="20">
-        <v>95.4198473282443</v>
-      </c>
-      <c r="C27" s="20">
-        <f t="shared" si="1"/>
-        <v>-0.0954198473282443</v>
-      </c>
-      <c r="F27" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G27" s="23">
-        <v>0.984344323774322</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25" spans="1:7">
-      <c r="A28" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="B28" s="20">
-        <v>100.796290696502</v>
-      </c>
-      <c r="C28" s="20">
-        <f t="shared" si="1"/>
-        <v>-0.100796290696502</v>
-      </c>
-      <c r="F28" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G28" s="23">
-        <v>0.954694884327784</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25" spans="1:7">
-      <c r="A29" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="B29" s="20">
-        <v>99.5024875621891</v>
-      </c>
-      <c r="C29" s="20">
-        <f t="shared" si="1"/>
-        <v>-0.0995024875621891</v>
-      </c>
-      <c r="F29" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G29" s="23">
-        <v>0.976404603726166</v>
-      </c>
-    </row>
-    <row r="30" ht="14.25" spans="1:7">
-      <c r="A30" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="B30" s="20">
-        <v>97.0873786407767</v>
-      </c>
-      <c r="C30" s="20">
-        <f t="shared" si="1"/>
-        <v>-0.0970873786407767</v>
-      </c>
-      <c r="F30" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G30" s="23">
-        <v>0.991395400914359</v>
-      </c>
-    </row>
-    <row r="31" ht="14.25" spans="1:7">
-      <c r="A31" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="B31" s="20">
-        <v>314.267756128221</v>
-      </c>
-      <c r="C31" s="20">
-        <f t="shared" ref="C31:C48" si="2">-B31/1000</f>
-        <v>-0.314267756128221</v>
-      </c>
-      <c r="F31" s="20">
-        <v>-0.3</v>
-      </c>
-      <c r="G31" s="23">
-        <v>0.965521196122588</v>
-      </c>
-    </row>
-    <row r="32" ht="14.25" spans="1:7">
-      <c r="A32" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="B32" s="20">
-        <v>304.692260816575</v>
-      </c>
-      <c r="C32" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.304692260816575</v>
-      </c>
-      <c r="F32" s="20">
-        <v>-0.3</v>
-      </c>
-      <c r="G32" s="24">
-        <v>2.03626250365614</v>
-      </c>
-    </row>
-    <row r="33" ht="14.25" spans="1:7">
-      <c r="A33" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="B33" s="20">
-        <v>293.427230046948</v>
-      </c>
-      <c r="C33" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.293427230046948</v>
-      </c>
-      <c r="F33" s="20">
-        <v>-0.3</v>
-      </c>
-      <c r="G33" s="23">
-        <v>0.992055264033481</v>
-      </c>
-    </row>
-    <row r="34" ht="14.25" spans="1:7">
-      <c r="A34" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="B34" s="26">
-        <v>296.73590504451</v>
-      </c>
-      <c r="C34" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.29673590504451</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="F34" s="20">
-        <v>-0.3</v>
-      </c>
-      <c r="G34" s="23">
-        <v>0.996409927774611</v>
-      </c>
-    </row>
-    <row r="35" ht="14.25" spans="1:7">
-      <c r="A35" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="B35" s="26">
-        <v>296.73590504451</v>
-      </c>
-      <c r="C35" s="27">
-        <f t="shared" si="2"/>
-        <v>-0.29673590504451</v>
-      </c>
-      <c r="F35" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="G35" s="23">
-        <v>0.990366511511847</v>
-      </c>
-    </row>
-    <row r="36" ht="14.25" spans="1:7">
-      <c r="A36" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="B36" s="20">
-        <v>293.427230046948</v>
-      </c>
-      <c r="C36" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.293427230046948</v>
-      </c>
-      <c r="F36" s="20">
-        <v>-0.3</v>
-      </c>
-      <c r="G36" s="23">
-        <v>1.00101116548929</v>
-      </c>
-    </row>
-    <row r="37" ht="14.25" spans="1:7">
-      <c r="A37" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="B37" s="20">
-        <v>285.225328009127</v>
-      </c>
-      <c r="C37" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.285225328009127</v>
-      </c>
-      <c r="F37" s="20">
-        <v>-0.3</v>
-      </c>
-      <c r="G37" s="23">
-        <v>1.04690459254695</v>
-      </c>
-    </row>
-    <row r="38" ht="14.25" spans="1:7">
-      <c r="A38" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="B38" s="20">
-        <v>314.267756128221</v>
-      </c>
-      <c r="C38" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.314267756128221</v>
-      </c>
-      <c r="F38" s="20">
-        <v>-0.3</v>
-      </c>
-      <c r="G38" s="23">
-        <v>0.95124107406349</v>
-      </c>
-    </row>
-    <row r="39" ht="14.25" spans="1:7">
-      <c r="A39" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="B39" s="20">
-        <v>100.78613182826</v>
-      </c>
-      <c r="C39" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.10078613182826</v>
-      </c>
-      <c r="F39" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G39" s="23">
-        <v>0.786490532132579</v>
-      </c>
-    </row>
-    <row r="40" ht="14.25" spans="1:7">
-      <c r="A40" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="B40" s="20">
-        <v>99.5421063109695</v>
-      </c>
-      <c r="C40" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.0995421063109695</v>
-      </c>
-      <c r="F40" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G40" s="23">
-        <v>1.00513452816592</v>
-      </c>
-    </row>
-    <row r="41" ht="14.25" spans="1:7">
-      <c r="A41" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="B41" s="20">
-        <v>98.9119683481701</v>
-      </c>
-      <c r="C41" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.0989119683481701</v>
-      </c>
-      <c r="F41" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G41" s="23">
-        <v>1.0189075012981</v>
-      </c>
-    </row>
-    <row r="42" ht="14.25" spans="1:7">
-      <c r="A42" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B42" s="20">
-        <v>98.9119683481701</v>
-      </c>
-      <c r="C42" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.0989119683481701</v>
-      </c>
-      <c r="F42" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G42" s="23">
-        <v>-0.00148210066326318</v>
-      </c>
-    </row>
-    <row r="43" ht="14.25" spans="1:7">
-      <c r="A43" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="B43" s="20">
-        <v>98.9119683481701</v>
-      </c>
-      <c r="C43" s="20">
-        <f t="shared" si="2"/>
-        <v>-0.0989119683481701</v>
-      </c>
-      <c r="F43" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G43" s="23">
-        <v>1.04013828913163</v>
-      </c>
-    </row>
-    <row r="44" ht="14.25" spans="1:7">
+      <c r="D43" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="20" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B44" s="20">
         <v>102.732689541812</v>
       </c>
       <c r="C44" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-0.102732689541812</v>
       </c>
-      <c r="F44" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G44" s="23">
-        <v>1.00120686910651</v>
-      </c>
-    </row>
-    <row r="45" ht="14.25" spans="1:7">
+      <c r="D44" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="20" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B45" s="20">
         <v>98.9119683481701</v>
       </c>
-      <c r="C45" s="27">
+      <c r="C45" s="24">
         <v>-0.1</v>
       </c>
-      <c r="F45" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G45" s="23">
-        <v>0.00585427974686723</v>
-      </c>
-    </row>
-    <row r="46" ht="14.25" spans="1:7">
+      <c r="D45" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="20" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B46" s="20">
         <v>104.733975701718</v>
@@ -4515,16 +4541,13 @@
         <f>-B45/1000</f>
         <v>-0.0989119683481701</v>
       </c>
-      <c r="F46" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G46" s="23">
-        <v>1.042062362991</v>
-      </c>
-    </row>
-    <row r="47" ht="14.25" spans="1:7">
+      <c r="D46" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="20" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B47" s="20">
         <v>97.1250971250971</v>
@@ -4533,16 +4556,13 @@
         <f>-B46/1000</f>
         <v>-0.104733975701718</v>
       </c>
-      <c r="F47" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G47" s="23">
-        <v>0.979760564664813</v>
-      </c>
-    </row>
-    <row r="48" ht="14.25" spans="1:7">
+      <c r="D47" s="21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="20" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B48" s="20">
         <v>100</v>
@@ -4551,11 +4571,8 @@
         <f>-B47/1000</f>
         <v>-0.0971250971250971</v>
       </c>
-      <c r="F48" s="20">
-        <v>-0.1</v>
-      </c>
-      <c r="G48" s="23">
-        <v>1.0710899688599</v>
+      <c r="D48" s="21">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -4588,39 +4605,39 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D2" s="4">
         <f t="shared" ref="D2:D12" si="0">100/4</f>
@@ -4630,22 +4647,22 @@
         <v>2.5</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" si="0"/>
@@ -4657,18 +4674,18 @@
       <c r="F3" s="7"/>
       <c r="G3" s="8"/>
       <c r="H3" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" si="0"/>
@@ -4680,18 +4697,18 @@
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
       <c r="H4" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="0"/>
@@ -4703,18 +4720,18 @@
       <c r="F5" s="7"/>
       <c r="G5" s="8"/>
       <c r="H5" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" si="0"/>
@@ -4726,18 +4743,18 @@
       <c r="F6" s="7"/>
       <c r="G6" s="8"/>
       <c r="H6" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
@@ -4749,18 +4766,18 @@
       <c r="F7" s="7"/>
       <c r="G7" s="8"/>
       <c r="H7" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
@@ -4772,18 +4789,18 @@
       <c r="F8" s="7"/>
       <c r="G8" s="8"/>
       <c r="H8" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
@@ -4795,18 +4812,18 @@
       <c r="F9" s="7"/>
       <c r="G9" s="8"/>
       <c r="H9" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
@@ -4818,18 +4835,18 @@
       <c r="F10" s="7"/>
       <c r="G10" s="8"/>
       <c r="H10" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:8">
       <c r="A11" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="0"/>
@@ -4841,18 +4858,18 @@
       <c r="F11" s="7"/>
       <c r="G11" s="8"/>
       <c r="H11" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="0"/>
@@ -4864,16 +4881,16 @@
       <c r="F12" s="9"/>
       <c r="G12" s="10"/>
       <c r="H12" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:8">
       <c r="A13" s="11" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D13" s="12">
         <f>100/2</f>
@@ -4883,52 +4900,52 @@
         <v>5</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="11"/>
     </row>
     <row r="14" customHeight="1" spans="1:8">
       <c r="A14" s="11" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="15" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="11"/>
     </row>
     <row r="15" customHeight="1" spans="1:8">
       <c r="A15" s="11" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="11" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="15" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="11"/>
     </row>
     <row r="16" customHeight="1" spans="1:8">
       <c r="A16" s="17" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D16" s="18">
         <f t="shared" ref="D16:D32" si="1">E16*7</f>
@@ -4948,13 +4965,13 @@
     </row>
     <row r="17" customHeight="1" spans="1:8">
       <c r="A17" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>206</v>
-      </c>
       <c r="C17" s="17" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D17" s="18">
         <f t="shared" si="1"/>
@@ -4974,13 +4991,13 @@
     </row>
     <row r="18" customHeight="1" spans="1:8">
       <c r="A18" s="17" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D18" s="18">
         <f t="shared" si="1"/>
@@ -5000,13 +5017,13 @@
     </row>
     <row r="19" customHeight="1" spans="1:8">
       <c r="A19" s="17" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D19" s="18">
         <f t="shared" si="1"/>
@@ -5026,13 +5043,13 @@
     </row>
     <row r="20" customHeight="1" spans="1:8">
       <c r="A20" s="17" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D20" s="18">
         <f t="shared" si="1"/>
@@ -5052,13 +5069,13 @@
     </row>
     <row r="21" customHeight="1" spans="1:8">
       <c r="A21" s="17" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D21" s="18">
         <f t="shared" si="1"/>
@@ -5078,13 +5095,13 @@
     </row>
     <row r="22" customHeight="1" spans="1:8">
       <c r="A22" s="17" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D22" s="18">
         <f t="shared" si="1"/>
@@ -5104,13 +5121,13 @@
     </row>
     <row r="23" customHeight="1" spans="1:8">
       <c r="A23" s="17" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D23" s="18">
         <f t="shared" si="1"/>
@@ -5130,13 +5147,13 @@
     </row>
     <row r="24" customHeight="1" spans="1:8">
       <c r="A24" s="17" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D24" s="18">
         <f t="shared" si="1"/>
@@ -5156,13 +5173,13 @@
     </row>
     <row r="25" customHeight="1" spans="1:8">
       <c r="A25" s="17" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D25" s="18">
         <f t="shared" si="1"/>
@@ -5182,13 +5199,13 @@
     </row>
     <row r="26" customHeight="1" spans="1:8">
       <c r="A26" s="17" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D26" s="18">
         <f t="shared" si="1"/>
@@ -5205,18 +5222,18 @@
         <v>5</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="1:8">
       <c r="A27" s="17" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D27" s="18">
         <f t="shared" si="1"/>
@@ -5233,18 +5250,18 @@
         <v>2</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="28" customHeight="1" spans="1:8">
       <c r="A28" s="17" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D28" s="18">
         <f t="shared" si="1"/>
@@ -5261,18 +5278,18 @@
         <v>2</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="29" customHeight="1" spans="1:8">
       <c r="A29" s="17" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D29" s="18">
         <f t="shared" si="1"/>
@@ -5289,18 +5306,18 @@
         <v>100</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="30" customHeight="1" spans="1:8">
       <c r="A30" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>237</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>235</v>
       </c>
       <c r="D30" s="18">
         <f t="shared" si="1"/>
@@ -5317,16 +5334,16 @@
         <v>50</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" customHeight="1" spans="1:8">
       <c r="A31" s="11" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="11" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D31" s="12">
         <f t="shared" si="1"/>
@@ -5346,11 +5363,11 @@
     </row>
     <row r="32" customHeight="1" spans="1:8">
       <c r="A32" s="11" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="11" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D32" s="12">
         <f t="shared" si="1"/>
@@ -5370,13 +5387,13 @@
     </row>
     <row r="33" customHeight="1" spans="1:8">
       <c r="A33" s="19" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="12">
@@ -5393,13 +5410,13 @@
     </row>
     <row r="34" customHeight="1" spans="1:8">
       <c r="A34" s="19" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12">

</xml_diff>